<commit_message>
CashMemo module Tests for Web and Mobile
</commit_message>
<xml_diff>
--- a/tests/artifact/script/Mobile-CashMemo.xlsx
+++ b/tests/artifact/script/Mobile-CashMemo.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="841">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="878">
   <si>
     <t>target</t>
   </si>
@@ -2578,6 +2578,117 @@
   </si>
   <si>
     <t>click on Ok button to confirm the cash memo creation</t>
+  </si>
+  <si>
+    <t>verify the cash memo create success message</t>
+  </si>
+  <si>
+    <t>${cashmemo.create.success.message}</t>
+  </si>
+  <si>
+    <t>Create Cash Memo Successfull!</t>
+  </si>
+  <si>
+    <t>verify title of created cash memo</t>
+  </si>
+  <si>
+    <t>${cashmemo.created.title}</t>
+  </si>
+  <si>
+    <t>Cash Memo</t>
+  </si>
+  <si>
+    <t>fetch the cashmemo no</t>
+  </si>
+  <si>
+    <t>created.cashmemono</t>
+  </si>
+  <si>
+    <t>${created.cashmemo.no}</t>
+  </si>
+  <si>
+    <t>verify created cashmemo no</t>
+  </si>
+  <si>
+    <t>${created.cashmemono}</t>
+  </si>
+  <si>
+    <t>click on cash memo close button</t>
+  </si>
+  <si>
+    <t>${close.button}</t>
+  </si>
+  <si>
+    <t>click on back button to navigate cashmemo list</t>
+  </si>
+  <si>
+    <t>${back.button}</t>
+  </si>
+  <si>
+    <t>fetch the count of cashmemo list</t>
+  </si>
+  <si>
+    <t>listnum</t>
+  </si>
+  <si>
+    <t>${cashmemo.list}</t>
+  </si>
+  <si>
+    <t>fetch the values fron the list</t>
+  </si>
+  <si>
+    <t>cashmemono</t>
+  </si>
+  <si>
+    <t>initialize the counter variable with zero value</t>
+  </si>
+  <si>
+    <t>counter</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>repeatuntil to verify the cashmemo</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>-1</t>
+  </si>
+  <si>
+    <t>compare the counter and list number</t>
+  </si>
+  <si>
+    <t>${counter}</t>
+  </si>
+  <si>
+    <t>${listnum}</t>
+  </si>
+  <si>
+    <t>increment the counter value to iterate the loop</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>fetch the cashmemo no from the list</t>
+  </si>
+  <si>
+    <t>cashmemono.list</t>
+  </si>
+  <si>
+    <t>${cashmemono.xpath.part1}[${counter}]${cashmemono.xpath.part2}</t>
+  </si>
+  <si>
+    <t>verify the created cashmemo is displayed in the list</t>
+  </si>
+  <si>
+    <t>${cashmemono.list}</t>
+  </si>
+  <si>
+    <t>ProceedIf(${cashmemono.list}=${created.cashmemono})</t>
   </si>
   <si>
     <t>Create Purchase Cash Memo from Cash Memo page and fill the fields</t>
@@ -3317,7 +3428,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3432,12 +3543,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3508,8 +3622,8 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3521,10 +3635,6 @@
     </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -6582,7 +6692,7 @@
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
@@ -6732,7 +6842,7 @@
       <c r="E5" s="30" t="s">
         <v>748</v>
       </c>
-      <c r="F5" s="63" t="s">
+      <c r="F5" s="62" t="s">
         <v>749</v>
       </c>
       <c r="G5" s="30"/>
@@ -6747,7 +6857,7 @@
     </row>
     <row r="6" s="3" customFormat="1" ht="15.6" spans="1:15">
       <c r="A6" s="22"/>
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="63" t="s">
         <v>750</v>
       </c>
       <c r="C6" s="33" t="s">
@@ -6759,7 +6869,7 @@
       <c r="E6" s="30" t="s">
         <v>751</v>
       </c>
-      <c r="F6" s="65" t="s">
+      <c r="F6" s="64" t="s">
         <v>752</v>
       </c>
       <c r="G6" s="30"/>
@@ -6774,7 +6884,7 @@
     </row>
     <row r="7" s="4" customFormat="1" ht="42" customHeight="1" spans="1:15">
       <c r="A7" s="22"/>
-      <c r="B7" s="66"/>
+      <c r="B7" s="65"/>
       <c r="C7" s="28"/>
       <c r="D7" s="29"/>
       <c r="E7" s="29"/>
@@ -7046,7 +7156,7 @@
     </row>
     <row r="23" s="4" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A23" s="31"/>
-      <c r="B23" s="38"/>
+      <c r="B23" s="37"/>
       <c r="C23" s="33"/>
       <c r="D23" s="30"/>
       <c r="E23" s="30"/>
@@ -7064,7 +7174,7 @@
     <row r="24" s="1" customFormat="1" ht="24" customHeight="1" spans="2:15">
       <c r="B24" s="23"/>
       <c r="C24" s="33"/>
-      <c r="D24" s="62"/>
+      <c r="D24" s="38"/>
       <c r="E24" s="30"/>
       <c r="F24" s="29"/>
       <c r="G24" s="30"/>
@@ -7080,7 +7190,7 @@
     <row r="25" s="1" customFormat="1" ht="28" customHeight="1" spans="2:15">
       <c r="B25" s="23"/>
       <c r="C25" s="33"/>
-      <c r="D25" s="62"/>
+      <c r="D25" s="38"/>
       <c r="E25" s="30"/>
       <c r="F25" s="35"/>
       <c r="G25" s="30"/>
@@ -7114,7 +7224,7 @@
       <c r="B27" s="23"/>
       <c r="C27" s="33"/>
       <c r="D27" s="30"/>
-      <c r="E27" s="36"/>
+      <c r="E27" s="58"/>
       <c r="F27" s="32"/>
       <c r="G27" s="30"/>
       <c r="H27" s="30"/>
@@ -7131,7 +7241,7 @@
       <c r="B28" s="23"/>
       <c r="C28" s="33"/>
       <c r="D28" s="30"/>
-      <c r="E28" s="36"/>
+      <c r="E28" s="58"/>
       <c r="F28" s="35"/>
       <c r="G28" s="30"/>
       <c r="H28" s="30"/>
@@ -7148,7 +7258,7 @@
       <c r="B29" s="23"/>
       <c r="C29" s="33"/>
       <c r="D29" s="30"/>
-      <c r="E29" s="36"/>
+      <c r="E29" s="58"/>
       <c r="F29" s="32"/>
       <c r="G29" s="30"/>
       <c r="H29" s="30"/>
@@ -7165,7 +7275,7 @@
       <c r="B30" s="23"/>
       <c r="C30" s="28"/>
       <c r="D30" s="29"/>
-      <c r="E30" s="36"/>
+      <c r="E30" s="58"/>
       <c r="F30" s="32"/>
       <c r="G30" s="30"/>
       <c r="H30" s="30"/>
@@ -7180,12 +7290,12 @@
     <row r="31" ht="19" customHeight="1" spans="3:6">
       <c r="C31" s="28"/>
       <c r="D31" s="29"/>
-      <c r="F31" s="67"/>
+      <c r="F31" s="66"/>
     </row>
     <row r="32" ht="19" customHeight="1" spans="3:6">
       <c r="C32" s="28"/>
       <c r="D32" s="29"/>
-      <c r="F32" s="67"/>
+      <c r="F32" s="66"/>
     </row>
     <row r="33" ht="19" customHeight="1" spans="3:6">
       <c r="C33" s="28"/>
@@ -7200,7 +7310,7 @@
     <row r="35" ht="19" customHeight="1" spans="3:6">
       <c r="C35" s="28"/>
       <c r="D35" s="29"/>
-      <c r="F35" s="67"/>
+      <c r="F35" s="66"/>
     </row>
     <row r="36" ht="21" customHeight="1" spans="3:4">
       <c r="C36" s="28"/>
@@ -10217,7 +10327,7 @@
     </row>
     <row r="207" ht="23" customHeight="1" spans="1:15">
       <c r="A207" s="31"/>
-      <c r="B207" s="38"/>
+      <c r="B207" s="37"/>
       <c r="C207" s="28"/>
       <c r="D207" s="29"/>
       <c r="E207" s="29"/>
@@ -10234,7 +10344,7 @@
     </row>
     <row r="208" ht="23" customHeight="1" spans="1:15">
       <c r="A208" s="31"/>
-      <c r="B208" s="38"/>
+      <c r="B208" s="37"/>
       <c r="C208" s="28"/>
       <c r="D208" s="29"/>
       <c r="E208" s="29"/>
@@ -10251,7 +10361,7 @@
     </row>
     <row r="209" ht="23" customHeight="1" spans="1:15">
       <c r="A209" s="31"/>
-      <c r="B209" s="38"/>
+      <c r="B209" s="37"/>
       <c r="C209" s="28"/>
       <c r="D209" s="29"/>
       <c r="E209" s="29"/>
@@ -10268,7 +10378,7 @@
     </row>
     <row r="210" ht="23" customHeight="1" spans="1:15">
       <c r="A210" s="31"/>
-      <c r="B210" s="38"/>
+      <c r="B210" s="37"/>
       <c r="C210" s="28"/>
       <c r="D210" s="29"/>
       <c r="E210" s="29"/>
@@ -10285,7 +10395,7 @@
     </row>
     <row r="211" ht="23" customHeight="1" spans="1:15">
       <c r="A211" s="31"/>
-      <c r="B211" s="38"/>
+      <c r="B211" s="37"/>
       <c r="C211" s="28"/>
       <c r="D211" s="29"/>
       <c r="E211" s="29"/>
@@ -10302,7 +10412,7 @@
     </row>
     <row r="212" ht="23" customHeight="1" spans="1:15">
       <c r="A212" s="31"/>
-      <c r="B212" s="38"/>
+      <c r="B212" s="37"/>
       <c r="C212" s="28"/>
       <c r="D212" s="29"/>
       <c r="E212" s="29"/>
@@ -10319,7 +10429,7 @@
     </row>
     <row r="213" ht="23" customHeight="1" spans="1:15">
       <c r="A213" s="31"/>
-      <c r="B213" s="38"/>
+      <c r="B213" s="37"/>
       <c r="C213" s="28"/>
       <c r="D213" s="29"/>
       <c r="E213" s="29"/>
@@ -10336,7 +10446,7 @@
     </row>
     <row r="214" ht="23" customHeight="1" spans="1:15">
       <c r="A214" s="31"/>
-      <c r="B214" s="38"/>
+      <c r="B214" s="37"/>
       <c r="C214" s="28"/>
       <c r="D214" s="29"/>
       <c r="E214" s="29"/>
@@ -10353,7 +10463,7 @@
     </row>
     <row r="215" ht="23" customHeight="1" spans="1:15">
       <c r="A215" s="31"/>
-      <c r="B215" s="38"/>
+      <c r="B215" s="37"/>
       <c r="C215" s="28"/>
       <c r="D215" s="29"/>
       <c r="E215" s="29"/>
@@ -10370,7 +10480,7 @@
     </row>
     <row r="216" ht="23" customHeight="1" spans="1:15">
       <c r="A216" s="31"/>
-      <c r="B216" s="38"/>
+      <c r="B216" s="37"/>
       <c r="C216" s="28"/>
       <c r="D216" s="29"/>
       <c r="E216" s="29"/>
@@ -10387,7 +10497,7 @@
     </row>
     <row r="217" ht="23" customHeight="1" spans="1:15">
       <c r="A217" s="31"/>
-      <c r="B217" s="38"/>
+      <c r="B217" s="37"/>
       <c r="C217" s="28"/>
       <c r="D217" s="29"/>
       <c r="E217" s="29"/>
@@ -10404,7 +10514,7 @@
     </row>
     <row r="218" ht="23" customHeight="1" spans="1:15">
       <c r="A218" s="31"/>
-      <c r="B218" s="38"/>
+      <c r="B218" s="37"/>
       <c r="C218" s="28"/>
       <c r="D218" s="29"/>
       <c r="E218" s="29"/>
@@ -10421,7 +10531,7 @@
     </row>
     <row r="219" ht="23" customHeight="1" spans="1:15">
       <c r="A219" s="31"/>
-      <c r="B219" s="38"/>
+      <c r="B219" s="37"/>
       <c r="C219" s="28"/>
       <c r="D219" s="29"/>
       <c r="E219" s="29"/>
@@ -10438,7 +10548,7 @@
     </row>
     <row r="220" ht="23" customHeight="1" spans="1:15">
       <c r="A220" s="31"/>
-      <c r="B220" s="38"/>
+      <c r="B220" s="37"/>
       <c r="C220" s="28"/>
       <c r="D220" s="29"/>
       <c r="E220" s="29"/>
@@ -10455,7 +10565,7 @@
     </row>
     <row r="221" ht="23" customHeight="1" spans="1:15">
       <c r="A221" s="31"/>
-      <c r="B221" s="38"/>
+      <c r="B221" s="37"/>
       <c r="C221" s="28"/>
       <c r="D221" s="29"/>
       <c r="E221" s="29"/>
@@ -10472,7 +10582,7 @@
     </row>
     <row r="222" ht="23" customHeight="1" spans="1:15">
       <c r="A222" s="31"/>
-      <c r="B222" s="38"/>
+      <c r="B222" s="37"/>
       <c r="C222" s="28"/>
       <c r="D222" s="29"/>
       <c r="E222" s="29"/>
@@ -10489,7 +10599,7 @@
     </row>
     <row r="223" ht="23" customHeight="1" spans="1:15">
       <c r="A223" s="31"/>
-      <c r="B223" s="38"/>
+      <c r="B223" s="37"/>
       <c r="C223" s="28"/>
       <c r="D223" s="29"/>
       <c r="E223" s="29"/>
@@ -10506,7 +10616,7 @@
     </row>
     <row r="224" ht="23" customHeight="1" spans="1:15">
       <c r="A224" s="31"/>
-      <c r="B224" s="38"/>
+      <c r="B224" s="37"/>
       <c r="C224" s="28"/>
       <c r="D224" s="29"/>
       <c r="E224" s="29"/>
@@ -10523,7 +10633,7 @@
     </row>
     <row r="225" ht="23" customHeight="1" spans="1:15">
       <c r="A225" s="31"/>
-      <c r="B225" s="38"/>
+      <c r="B225" s="37"/>
       <c r="C225" s="28"/>
       <c r="D225" s="29"/>
       <c r="E225" s="29"/>
@@ -10650,12 +10760,12 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P308"/>
+  <dimension ref="A1:P306"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomLeft" activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
@@ -10668,7 +10778,7 @@
     <col min="6" max="6" width="42.5333333333333" style="9" customWidth="1"/>
     <col min="7" max="7" width="16.125" style="9" customWidth="1"/>
     <col min="8" max="9" width="9.25" style="9" customWidth="1"/>
-    <col min="10" max="10" width="28.6666666666667" style="10" customWidth="1"/>
+    <col min="10" max="10" width="51.2" style="10" customWidth="1"/>
     <col min="11" max="11" width="1.66666666666667" style="11" customWidth="1"/>
     <col min="12" max="12" width="12" style="12" customWidth="1"/>
     <col min="13" max="13" width="12.5" style="13" customWidth="1"/>
@@ -11729,11 +11839,21 @@
     </row>
     <row r="40" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A40" s="22"/>
-      <c r="B40" s="23"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="32"/>
+      <c r="B40" s="23" t="s">
+        <v>838</v>
+      </c>
+      <c r="C40" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" s="29" t="s">
+        <v>530</v>
+      </c>
+      <c r="E40" s="34" t="s">
+        <v>839</v>
+      </c>
+      <c r="F40" s="32" t="s">
+        <v>840</v>
+      </c>
       <c r="G40" s="30"/>
       <c r="H40" s="30"/>
       <c r="I40" s="30"/>
@@ -11746,11 +11866,21 @@
     </row>
     <row r="41" s="3" customFormat="1" ht="35" customHeight="1" spans="1:15">
       <c r="A41" s="22"/>
-      <c r="B41" s="23"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="58"/>
+      <c r="B41" s="23" t="s">
+        <v>841</v>
+      </c>
+      <c r="C41" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" s="30" t="s">
+        <v>530</v>
+      </c>
+      <c r="E41" s="29" t="s">
+        <v>842</v>
+      </c>
+      <c r="F41" s="36" t="s">
+        <v>843</v>
+      </c>
       <c r="G41" s="29"/>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
@@ -11761,47 +11891,77 @@
       <c r="N41" s="4"/>
       <c r="O41" s="25"/>
     </row>
-    <row r="42" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="42" s="3" customFormat="1" ht="35" customHeight="1" spans="1:15">
       <c r="A42" s="22"/>
-      <c r="B42" s="23"/>
-      <c r="C42" s="33"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="32"/>
+      <c r="B42" s="23" t="s">
+        <v>844</v>
+      </c>
+      <c r="C42" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" s="30" t="s">
+        <v>493</v>
+      </c>
+      <c r="E42" s="29" t="s">
+        <v>845</v>
+      </c>
+      <c r="F42" s="29" t="s">
+        <v>846</v>
+      </c>
       <c r="G42" s="29"/>
-      <c r="H42" s="30"/>
-      <c r="I42" s="30"/>
-      <c r="J42" s="35"/>
-      <c r="K42" s="25"/>
-      <c r="L42" s="26"/>
-      <c r="M42" s="24"/>
-      <c r="N42" s="26"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
       <c r="O42" s="25"/>
     </row>
     <row r="43" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A43" s="31"/>
-      <c r="B43" s="23"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="23" t="s">
+        <v>847</v>
+      </c>
+      <c r="C43" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43" s="29" t="s">
+        <v>530</v>
+      </c>
+      <c r="E43" s="29" t="s">
+        <v>846</v>
+      </c>
+      <c r="F43" s="32" t="s">
+        <v>848</v>
+      </c>
       <c r="G43" s="29"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="48"/>
-      <c r="K43" s="40"/>
-      <c r="L43" s="49"/>
-      <c r="M43" s="50"/>
-      <c r="N43" s="49"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="35"/>
+      <c r="K43" s="25"/>
+      <c r="L43" s="26"/>
+      <c r="M43" s="24"/>
+      <c r="N43" s="26"/>
       <c r="O43" s="25"/>
     </row>
     <row r="44" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A44" s="31"/>
-      <c r="B44" s="23"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
+      <c r="B44" s="23" t="s">
+        <v>849</v>
+      </c>
+      <c r="C44" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" s="29" t="s">
+        <v>576</v>
+      </c>
+      <c r="E44" s="29" t="s">
+        <v>850</v>
+      </c>
+      <c r="F44" s="29" t="s">
+        <v>752</v>
+      </c>
       <c r="G44" s="29"/>
       <c r="H44" s="29"/>
       <c r="I44" s="29"/>
@@ -11814,11 +11974,21 @@
     </row>
     <row r="45" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A45" s="31"/>
-      <c r="B45" s="38"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
+      <c r="B45" s="23" t="s">
+        <v>851</v>
+      </c>
+      <c r="C45" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="29" t="s">
+        <v>576</v>
+      </c>
+      <c r="E45" s="29" t="s">
+        <v>852</v>
+      </c>
+      <c r="F45" s="29" t="s">
+        <v>752</v>
+      </c>
       <c r="G45" s="29"/>
       <c r="H45" s="29"/>
       <c r="I45" s="29"/>
@@ -11831,11 +12001,21 @@
     </row>
     <row r="46" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A46" s="22"/>
-      <c r="B46" s="38"/>
-      <c r="C46" s="33"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="30"/>
-      <c r="F46" s="30"/>
+      <c r="B46" s="23" t="s">
+        <v>853</v>
+      </c>
+      <c r="C46" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" s="29" t="s">
+        <v>483</v>
+      </c>
+      <c r="E46" s="29" t="s">
+        <v>854</v>
+      </c>
+      <c r="F46" s="30" t="s">
+        <v>855</v>
+      </c>
       <c r="G46" s="29"/>
       <c r="H46" s="30"/>
       <c r="I46" s="30"/>
@@ -11848,11 +12028,21 @@
     </row>
     <row r="47" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A47" s="22"/>
-      <c r="B47" s="23"/>
-      <c r="C47" s="33"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="30"/>
+      <c r="B47" s="23" t="s">
+        <v>856</v>
+      </c>
+      <c r="C47" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" s="29" t="s">
+        <v>493</v>
+      </c>
+      <c r="E47" s="29" t="s">
+        <v>857</v>
+      </c>
+      <c r="F47" s="30" t="s">
+        <v>855</v>
+      </c>
       <c r="G47" s="29"/>
       <c r="H47" s="30"/>
       <c r="I47" s="30"/>
@@ -11865,11 +12055,21 @@
     </row>
     <row r="48" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A48" s="22"/>
-      <c r="B48" s="23"/>
-      <c r="C48" s="33"/>
-      <c r="D48" s="30"/>
-      <c r="E48" s="30"/>
-      <c r="F48" s="30"/>
+      <c r="B48" s="23" t="s">
+        <v>858</v>
+      </c>
+      <c r="C48" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="29" t="s">
+        <v>471</v>
+      </c>
+      <c r="E48" s="29" t="s">
+        <v>859</v>
+      </c>
+      <c r="F48" s="30" t="s">
+        <v>860</v>
+      </c>
       <c r="G48" s="29"/>
       <c r="H48" s="30"/>
       <c r="I48" s="30"/>
@@ -11881,46 +12081,76 @@
       <c r="O48" s="25"/>
     </row>
     <row r="49" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A49" s="22"/>
-      <c r="B49" s="23"/>
-      <c r="C49" s="33"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="30"/>
+      <c r="A49" s="31"/>
+      <c r="B49" s="23" t="s">
+        <v>861</v>
+      </c>
+      <c r="C49" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="30" t="s">
+        <v>465</v>
+      </c>
+      <c r="E49" s="30" t="s">
+        <v>862</v>
+      </c>
+      <c r="F49" s="35" t="s">
+        <v>863</v>
+      </c>
       <c r="G49" s="29"/>
-      <c r="H49" s="30"/>
-      <c r="I49" s="30"/>
-      <c r="J49" s="35"/>
-      <c r="K49" s="25"/>
-      <c r="L49" s="26"/>
-      <c r="M49" s="24"/>
-      <c r="N49" s="26"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="29"/>
+      <c r="J49" s="48"/>
+      <c r="K49" s="40"/>
+      <c r="L49" s="49"/>
+      <c r="M49" s="50"/>
+      <c r="N49" s="49"/>
       <c r="O49" s="25"/>
     </row>
     <row r="50" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A50" s="22"/>
-      <c r="B50" s="23"/>
-      <c r="C50" s="33"/>
-      <c r="D50" s="30"/>
-      <c r="E50" s="30"/>
-      <c r="F50" s="30"/>
+      <c r="A50" s="31"/>
+      <c r="B50" s="37" t="s">
+        <v>864</v>
+      </c>
+      <c r="C50" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="E50" s="30" t="s">
+        <v>865</v>
+      </c>
+      <c r="F50" s="29" t="s">
+        <v>866</v>
+      </c>
       <c r="G50" s="29"/>
-      <c r="H50" s="30"/>
-      <c r="I50" s="30"/>
-      <c r="J50" s="35"/>
-      <c r="K50" s="25"/>
-      <c r="L50" s="26"/>
-      <c r="M50" s="24"/>
-      <c r="N50" s="26"/>
+      <c r="H50" s="29"/>
+      <c r="I50" s="29"/>
+      <c r="J50" s="48"/>
+      <c r="K50" s="40"/>
+      <c r="L50" s="49"/>
+      <c r="M50" s="50"/>
+      <c r="N50" s="49"/>
       <c r="O50" s="25"/>
     </row>
     <row r="51" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A51" s="31"/>
-      <c r="B51" s="23"/>
-      <c r="C51" s="33"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="30"/>
-      <c r="F51" s="30"/>
+      <c r="B51" s="37" t="s">
+        <v>867</v>
+      </c>
+      <c r="C51" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D51" s="38" t="s">
+        <v>302</v>
+      </c>
+      <c r="E51" s="30" t="s">
+        <v>859</v>
+      </c>
+      <c r="F51" s="35" t="s">
+        <v>868</v>
+      </c>
       <c r="G51" s="29"/>
       <c r="H51" s="29"/>
       <c r="I51" s="29"/>
@@ -11933,11 +12163,21 @@
     </row>
     <row r="52" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A52" s="31"/>
-      <c r="B52" s="38"/>
-      <c r="C52" s="28"/>
-      <c r="D52" s="29"/>
-      <c r="E52" s="29"/>
-      <c r="F52" s="29"/>
+      <c r="B52" s="37" t="s">
+        <v>869</v>
+      </c>
+      <c r="C52" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52" s="29" t="s">
+        <v>493</v>
+      </c>
+      <c r="E52" s="29" t="s">
+        <v>870</v>
+      </c>
+      <c r="F52" s="32" t="s">
+        <v>871</v>
+      </c>
       <c r="G52" s="29"/>
       <c r="H52" s="29"/>
       <c r="I52" s="29"/>
@@ -11950,15 +12190,27 @@
     </row>
     <row r="53" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A53" s="31"/>
-      <c r="B53" s="38"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="29"/>
-      <c r="F53" s="29"/>
+      <c r="B53" s="37" t="s">
+        <v>872</v>
+      </c>
+      <c r="C53" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="E53" s="29" t="s">
+        <v>873</v>
+      </c>
+      <c r="F53" s="32" t="s">
+        <v>848</v>
+      </c>
       <c r="G53" s="29"/>
       <c r="H53" s="29"/>
       <c r="I53" s="29"/>
-      <c r="J53" s="48"/>
+      <c r="J53" s="48" t="s">
+        <v>874</v>
+      </c>
       <c r="K53" s="40"/>
       <c r="L53" s="49"/>
       <c r="M53" s="50"/>
@@ -11967,11 +12219,11 @@
     </row>
     <row r="54" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A54" s="31"/>
-      <c r="B54" s="38"/>
-      <c r="C54" s="28"/>
-      <c r="D54" s="29"/>
+      <c r="B54" s="37"/>
+      <c r="C54" s="33"/>
+      <c r="D54" s="30"/>
       <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
+      <c r="F54" s="30"/>
       <c r="G54" s="29"/>
       <c r="H54" s="29"/>
       <c r="I54" s="29"/>
@@ -11984,7 +12236,7 @@
     </row>
     <row r="55" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A55" s="31"/>
-      <c r="B55" s="38"/>
+      <c r="B55" s="37"/>
       <c r="C55" s="28"/>
       <c r="D55" s="29"/>
       <c r="E55" s="29"/>
@@ -12001,7 +12253,7 @@
     </row>
     <row r="56" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A56" s="31"/>
-      <c r="B56" s="38"/>
+      <c r="B56" s="37"/>
       <c r="C56" s="33"/>
       <c r="D56" s="30"/>
       <c r="E56" s="30"/>
@@ -12018,7 +12270,7 @@
     </row>
     <row r="57" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A57" s="31"/>
-      <c r="B57" s="38"/>
+      <c r="B57" s="37"/>
       <c r="C57" s="28"/>
       <c r="D57" s="29"/>
       <c r="E57" s="29"/>
@@ -12035,7 +12287,7 @@
     </row>
     <row r="58" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A58" s="31"/>
-      <c r="B58" s="38"/>
+      <c r="B58" s="37"/>
       <c r="C58" s="33"/>
       <c r="D58" s="30"/>
       <c r="E58" s="30"/>
@@ -12052,7 +12304,7 @@
     </row>
     <row r="59" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A59" s="31"/>
-      <c r="B59" s="38"/>
+      <c r="B59" s="37"/>
       <c r="C59" s="28"/>
       <c r="D59" s="29"/>
       <c r="E59" s="29"/>
@@ -12069,7 +12321,7 @@
     </row>
     <row r="60" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A60" s="31"/>
-      <c r="B60" s="38"/>
+      <c r="B60" s="37"/>
       <c r="C60" s="33"/>
       <c r="D60" s="30"/>
       <c r="E60" s="30"/>
@@ -12086,11 +12338,11 @@
     </row>
     <row r="61" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A61" s="31"/>
-      <c r="B61" s="38"/>
-      <c r="C61" s="28"/>
-      <c r="D61" s="29"/>
+      <c r="B61" s="37"/>
+      <c r="C61" s="33"/>
+      <c r="D61" s="30"/>
       <c r="E61" s="29"/>
-      <c r="F61" s="29"/>
+      <c r="F61" s="30"/>
       <c r="G61" s="29"/>
       <c r="H61" s="29"/>
       <c r="I61" s="29"/>
@@ -12103,11 +12355,11 @@
     </row>
     <row r="62" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A62" s="31"/>
-      <c r="B62" s="38"/>
-      <c r="C62" s="33"/>
-      <c r="D62" s="30"/>
-      <c r="E62" s="30"/>
-      <c r="F62" s="30"/>
+      <c r="B62" s="37"/>
+      <c r="C62" s="28"/>
+      <c r="D62" s="29"/>
+      <c r="E62" s="29"/>
+      <c r="F62" s="29"/>
       <c r="G62" s="29"/>
       <c r="H62" s="29"/>
       <c r="I62" s="29"/>
@@ -12120,11 +12372,11 @@
     </row>
     <row r="63" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A63" s="31"/>
-      <c r="B63" s="38"/>
-      <c r="C63" s="33"/>
-      <c r="D63" s="30"/>
+      <c r="B63" s="37"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="29"/>
       <c r="E63" s="29"/>
-      <c r="F63" s="30"/>
+      <c r="F63" s="29"/>
       <c r="G63" s="29"/>
       <c r="H63" s="29"/>
       <c r="I63" s="29"/>
@@ -12137,7 +12389,7 @@
     </row>
     <row r="64" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A64" s="31"/>
-      <c r="B64" s="38"/>
+      <c r="B64" s="37"/>
       <c r="C64" s="28"/>
       <c r="D64" s="29"/>
       <c r="E64" s="29"/>
@@ -12154,11 +12406,11 @@
     </row>
     <row r="65" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A65" s="31"/>
-      <c r="B65" s="38"/>
-      <c r="C65" s="28"/>
-      <c r="D65" s="29"/>
-      <c r="E65" s="29"/>
-      <c r="F65" s="29"/>
+      <c r="B65" s="37"/>
+      <c r="C65" s="33"/>
+      <c r="D65" s="30"/>
+      <c r="E65" s="30"/>
+      <c r="F65" s="30"/>
       <c r="G65" s="29"/>
       <c r="H65" s="29"/>
       <c r="I65" s="29"/>
@@ -12171,11 +12423,11 @@
     </row>
     <row r="66" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A66" s="31"/>
-      <c r="B66" s="38"/>
+      <c r="B66" s="37"/>
       <c r="C66" s="28"/>
       <c r="D66" s="29"/>
       <c r="E66" s="29"/>
-      <c r="F66" s="29"/>
+      <c r="F66" s="14"/>
       <c r="G66" s="29"/>
       <c r="H66" s="29"/>
       <c r="I66" s="29"/>
@@ -12188,11 +12440,11 @@
     </row>
     <row r="67" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A67" s="31"/>
-      <c r="B67" s="38"/>
-      <c r="C67" s="33"/>
-      <c r="D67" s="30"/>
-      <c r="E67" s="30"/>
-      <c r="F67" s="30"/>
+      <c r="B67" s="37"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="29"/>
+      <c r="E67" s="29"/>
+      <c r="F67" s="29"/>
       <c r="G67" s="29"/>
       <c r="H67" s="29"/>
       <c r="I67" s="29"/>
@@ -12205,7 +12457,7 @@
     </row>
     <row r="68" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A68" s="31"/>
-      <c r="B68" s="38"/>
+      <c r="B68" s="37"/>
       <c r="C68" s="28"/>
       <c r="D68" s="29"/>
       <c r="E68" s="29"/>
@@ -12222,11 +12474,11 @@
     </row>
     <row r="69" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A69" s="31"/>
-      <c r="B69" s="38"/>
-      <c r="C69" s="28"/>
-      <c r="D69" s="29"/>
-      <c r="E69" s="29"/>
-      <c r="F69" s="29"/>
+      <c r="B69" s="37"/>
+      <c r="C69" s="33"/>
+      <c r="D69" s="30"/>
+      <c r="E69" s="30"/>
+      <c r="F69" s="30"/>
       <c r="G69" s="29"/>
       <c r="H69" s="29"/>
       <c r="I69" s="29"/>
@@ -12239,11 +12491,11 @@
     </row>
     <row r="70" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A70" s="31"/>
-      <c r="B70" s="38"/>
+      <c r="B70" s="37"/>
       <c r="C70" s="28"/>
       <c r="D70" s="29"/>
       <c r="E70" s="29"/>
-      <c r="F70" s="14"/>
+      <c r="F70" s="30"/>
       <c r="G70" s="29"/>
       <c r="H70" s="29"/>
       <c r="I70" s="29"/>
@@ -12256,10 +12508,10 @@
     </row>
     <row r="71" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A71" s="31"/>
-      <c r="B71" s="38"/>
-      <c r="C71" s="33"/>
-      <c r="D71" s="30"/>
-      <c r="E71" s="30"/>
+      <c r="B71" s="37"/>
+      <c r="C71" s="28"/>
+      <c r="D71" s="29"/>
+      <c r="E71" s="29"/>
       <c r="F71" s="30"/>
       <c r="G71" s="29"/>
       <c r="H71" s="29"/>
@@ -12273,7 +12525,7 @@
     </row>
     <row r="72" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A72" s="31"/>
-      <c r="B72" s="38"/>
+      <c r="B72" s="37"/>
       <c r="C72" s="28"/>
       <c r="D72" s="29"/>
       <c r="E72" s="29"/>
@@ -12290,11 +12542,11 @@
     </row>
     <row r="73" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A73" s="31"/>
-      <c r="B73" s="38"/>
+      <c r="B73" s="37"/>
       <c r="C73" s="28"/>
       <c r="D73" s="29"/>
       <c r="E73" s="29"/>
-      <c r="F73" s="30"/>
+      <c r="F73" s="29"/>
       <c r="G73" s="29"/>
       <c r="H73" s="29"/>
       <c r="I73" s="29"/>
@@ -12307,10 +12559,10 @@
     </row>
     <row r="74" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A74" s="31"/>
-      <c r="B74" s="38"/>
-      <c r="C74" s="28"/>
-      <c r="D74" s="29"/>
-      <c r="E74" s="29"/>
+      <c r="B74" s="37"/>
+      <c r="C74" s="33"/>
+      <c r="D74" s="30"/>
+      <c r="E74" s="30"/>
       <c r="F74" s="30"/>
       <c r="G74" s="29"/>
       <c r="H74" s="29"/>
@@ -12324,7 +12576,7 @@
     </row>
     <row r="75" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A75" s="31"/>
-      <c r="B75" s="38"/>
+      <c r="B75" s="37"/>
       <c r="C75" s="28"/>
       <c r="D75" s="29"/>
       <c r="E75" s="29"/>
@@ -12341,7 +12593,7 @@
     </row>
     <row r="76" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A76" s="31"/>
-      <c r="B76" s="38"/>
+      <c r="B76" s="37"/>
       <c r="C76" s="33"/>
       <c r="D76" s="30"/>
       <c r="E76" s="30"/>
@@ -12358,7 +12610,7 @@
     </row>
     <row r="77" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A77" s="31"/>
-      <c r="B77" s="38"/>
+      <c r="B77" s="37"/>
       <c r="C77" s="28"/>
       <c r="D77" s="29"/>
       <c r="E77" s="29"/>
@@ -12375,7 +12627,7 @@
     </row>
     <row r="78" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A78" s="31"/>
-      <c r="B78" s="38"/>
+      <c r="B78" s="37"/>
       <c r="C78" s="33"/>
       <c r="D78" s="30"/>
       <c r="E78" s="30"/>
@@ -12392,11 +12644,11 @@
     </row>
     <row r="79" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A79" s="31"/>
-      <c r="B79" s="38"/>
-      <c r="C79" s="28"/>
-      <c r="D79" s="29"/>
+      <c r="B79" s="37"/>
+      <c r="C79" s="33"/>
+      <c r="D79" s="30"/>
       <c r="E79" s="29"/>
-      <c r="F79" s="29"/>
+      <c r="F79" s="30"/>
       <c r="G79" s="29"/>
       <c r="H79" s="29"/>
       <c r="I79" s="29"/>
@@ -12409,11 +12661,11 @@
     </row>
     <row r="80" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A80" s="31"/>
-      <c r="B80" s="38"/>
-      <c r="C80" s="33"/>
-      <c r="D80" s="30"/>
-      <c r="E80" s="30"/>
-      <c r="F80" s="30"/>
+      <c r="B80" s="37"/>
+      <c r="C80" s="28"/>
+      <c r="D80" s="29"/>
+      <c r="E80" s="29"/>
+      <c r="F80" s="29"/>
       <c r="G80" s="29"/>
       <c r="H80" s="29"/>
       <c r="I80" s="29"/>
@@ -12426,11 +12678,11 @@
     </row>
     <row r="81" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A81" s="31"/>
-      <c r="B81" s="38"/>
-      <c r="C81" s="33"/>
-      <c r="D81" s="30"/>
+      <c r="B81" s="37"/>
+      <c r="C81" s="28"/>
+      <c r="D81" s="29"/>
       <c r="E81" s="29"/>
-      <c r="F81" s="30"/>
+      <c r="F81" s="29"/>
       <c r="G81" s="29"/>
       <c r="H81" s="29"/>
       <c r="I81" s="29"/>
@@ -12443,7 +12695,7 @@
     </row>
     <row r="82" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A82" s="31"/>
-      <c r="B82" s="38"/>
+      <c r="B82" s="37"/>
       <c r="C82" s="28"/>
       <c r="D82" s="29"/>
       <c r="E82" s="29"/>
@@ -12460,7 +12712,7 @@
     </row>
     <row r="83" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A83" s="31"/>
-      <c r="B83" s="38"/>
+      <c r="B83" s="37"/>
       <c r="C83" s="28"/>
       <c r="D83" s="29"/>
       <c r="E83" s="29"/>
@@ -12477,7 +12729,7 @@
     </row>
     <row r="84" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A84" s="31"/>
-      <c r="B84" s="38"/>
+      <c r="B84" s="37"/>
       <c r="C84" s="28"/>
       <c r="D84" s="29"/>
       <c r="E84" s="29"/>
@@ -12494,7 +12746,7 @@
     </row>
     <row r="85" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A85" s="31"/>
-      <c r="B85" s="38"/>
+      <c r="B85" s="37"/>
       <c r="C85" s="28"/>
       <c r="D85" s="29"/>
       <c r="E85" s="29"/>
@@ -12511,7 +12763,7 @@
     </row>
     <row r="86" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A86" s="31"/>
-      <c r="B86" s="38"/>
+      <c r="B86" s="37"/>
       <c r="C86" s="28"/>
       <c r="D86" s="29"/>
       <c r="E86" s="29"/>
@@ -12528,7 +12780,7 @@
     </row>
     <row r="87" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A87" s="31"/>
-      <c r="B87" s="38"/>
+      <c r="B87" s="37"/>
       <c r="C87" s="28"/>
       <c r="D87" s="29"/>
       <c r="E87" s="29"/>
@@ -12545,7 +12797,7 @@
     </row>
     <row r="88" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A88" s="31"/>
-      <c r="B88" s="38"/>
+      <c r="B88" s="37"/>
       <c r="C88" s="28"/>
       <c r="D88" s="29"/>
       <c r="E88" s="29"/>
@@ -12562,7 +12814,7 @@
     </row>
     <row r="89" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A89" s="31"/>
-      <c r="B89" s="38"/>
+      <c r="B89" s="37"/>
       <c r="C89" s="28"/>
       <c r="D89" s="29"/>
       <c r="E89" s="29"/>
@@ -12579,12 +12831,11 @@
     </row>
     <row r="90" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A90" s="31"/>
-      <c r="B90" s="38"/>
+      <c r="B90" s="37"/>
       <c r="C90" s="28"/>
       <c r="D90" s="29"/>
       <c r="E90" s="29"/>
       <c r="F90" s="29"/>
-      <c r="G90" s="29"/>
       <c r="H90" s="29"/>
       <c r="I90" s="29"/>
       <c r="J90" s="48"/>
@@ -12596,12 +12847,11 @@
     </row>
     <row r="91" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A91" s="31"/>
-      <c r="B91" s="38"/>
+      <c r="B91" s="37"/>
       <c r="C91" s="28"/>
       <c r="D91" s="29"/>
       <c r="E91" s="29"/>
       <c r="F91" s="29"/>
-      <c r="G91" s="29"/>
       <c r="H91" s="29"/>
       <c r="I91" s="29"/>
       <c r="J91" s="48"/>
@@ -12613,11 +12863,12 @@
     </row>
     <row r="92" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A92" s="31"/>
-      <c r="B92" s="38"/>
+      <c r="B92" s="37"/>
       <c r="C92" s="28"/>
       <c r="D92" s="29"/>
       <c r="E92" s="29"/>
       <c r="F92" s="29"/>
+      <c r="G92" s="29"/>
       <c r="H92" s="29"/>
       <c r="I92" s="29"/>
       <c r="J92" s="48"/>
@@ -12629,11 +12880,12 @@
     </row>
     <row r="93" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A93" s="31"/>
-      <c r="B93" s="38"/>
+      <c r="B93" s="37"/>
       <c r="C93" s="28"/>
       <c r="D93" s="29"/>
       <c r="E93" s="29"/>
-      <c r="F93" s="29"/>
+      <c r="F93" s="30"/>
+      <c r="G93" s="29"/>
       <c r="H93" s="29"/>
       <c r="I93" s="29"/>
       <c r="J93" s="48"/>
@@ -12645,11 +12897,11 @@
     </row>
     <row r="94" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A94" s="31"/>
-      <c r="B94" s="38"/>
+      <c r="B94" s="37"/>
       <c r="C94" s="28"/>
       <c r="D94" s="29"/>
       <c r="E94" s="29"/>
-      <c r="F94" s="29"/>
+      <c r="F94" s="30"/>
       <c r="G94" s="29"/>
       <c r="H94" s="29"/>
       <c r="I94" s="29"/>
@@ -12662,7 +12914,7 @@
     </row>
     <row r="95" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A95" s="31"/>
-      <c r="B95" s="38"/>
+      <c r="B95" s="37"/>
       <c r="C95" s="28"/>
       <c r="D95" s="29"/>
       <c r="E95" s="29"/>
@@ -12679,11 +12931,11 @@
     </row>
     <row r="96" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A96" s="31"/>
-      <c r="B96" s="38"/>
+      <c r="B96" s="37"/>
       <c r="C96" s="28"/>
       <c r="D96" s="29"/>
       <c r="E96" s="29"/>
-      <c r="F96" s="30"/>
+      <c r="F96" s="29"/>
       <c r="G96" s="29"/>
       <c r="H96" s="29"/>
       <c r="I96" s="29"/>
@@ -12696,10 +12948,10 @@
     </row>
     <row r="97" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A97" s="31"/>
-      <c r="B97" s="38"/>
-      <c r="C97" s="28"/>
-      <c r="D97" s="29"/>
-      <c r="E97" s="29"/>
+      <c r="B97" s="37"/>
+      <c r="C97" s="33"/>
+      <c r="D97" s="30"/>
+      <c r="E97" s="30"/>
       <c r="F97" s="30"/>
       <c r="G97" s="29"/>
       <c r="H97" s="29"/>
@@ -12713,11 +12965,11 @@
     </row>
     <row r="98" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A98" s="31"/>
-      <c r="B98" s="38"/>
-      <c r="C98" s="28"/>
-      <c r="D98" s="29"/>
+      <c r="B98" s="37"/>
+      <c r="C98" s="33"/>
+      <c r="D98" s="30"/>
       <c r="E98" s="29"/>
-      <c r="F98" s="29"/>
+      <c r="F98" s="30"/>
       <c r="G98" s="29"/>
       <c r="H98" s="29"/>
       <c r="I98" s="29"/>
@@ -12730,11 +12982,11 @@
     </row>
     <row r="99" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A99" s="31"/>
-      <c r="B99" s="38"/>
-      <c r="C99" s="33"/>
-      <c r="D99" s="30"/>
-      <c r="E99" s="30"/>
-      <c r="F99" s="30"/>
+      <c r="B99" s="37"/>
+      <c r="C99" s="28"/>
+      <c r="D99" s="29"/>
+      <c r="E99" s="29"/>
+      <c r="F99" s="29"/>
       <c r="G99" s="29"/>
       <c r="H99" s="29"/>
       <c r="I99" s="29"/>
@@ -12747,11 +12999,11 @@
     </row>
     <row r="100" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A100" s="31"/>
-      <c r="B100" s="38"/>
-      <c r="C100" s="33"/>
-      <c r="D100" s="30"/>
+      <c r="B100" s="37"/>
+      <c r="C100" s="28"/>
+      <c r="D100" s="29"/>
       <c r="E100" s="29"/>
-      <c r="F100" s="30"/>
+      <c r="F100" s="29"/>
       <c r="G100" s="29"/>
       <c r="H100" s="29"/>
       <c r="I100" s="29"/>
@@ -12764,7 +13016,7 @@
     </row>
     <row r="101" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A101" s="31"/>
-      <c r="B101" s="38"/>
+      <c r="B101" s="37"/>
       <c r="C101" s="28"/>
       <c r="D101" s="29"/>
       <c r="E101" s="29"/>
@@ -12781,7 +13033,7 @@
     </row>
     <row r="102" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A102" s="31"/>
-      <c r="B102" s="38"/>
+      <c r="B102" s="37"/>
       <c r="C102" s="28"/>
       <c r="D102" s="29"/>
       <c r="E102" s="29"/>
@@ -12798,7 +13050,7 @@
     </row>
     <row r="103" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A103" s="31"/>
-      <c r="B103" s="38"/>
+      <c r="B103" s="37"/>
       <c r="C103" s="28"/>
       <c r="D103" s="29"/>
       <c r="E103" s="29"/>
@@ -12815,7 +13067,7 @@
     </row>
     <row r="104" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A104" s="31"/>
-      <c r="B104" s="38"/>
+      <c r="B104" s="37"/>
       <c r="C104" s="28"/>
       <c r="D104" s="29"/>
       <c r="E104" s="29"/>
@@ -12832,11 +13084,11 @@
     </row>
     <row r="105" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A105" s="31"/>
-      <c r="B105" s="38"/>
+      <c r="B105" s="37"/>
       <c r="C105" s="28"/>
       <c r="D105" s="29"/>
       <c r="E105" s="29"/>
-      <c r="F105" s="29"/>
+      <c r="F105" s="30"/>
       <c r="G105" s="29"/>
       <c r="H105" s="29"/>
       <c r="I105" s="29"/>
@@ -12849,11 +13101,11 @@
     </row>
     <row r="106" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A106" s="31"/>
-      <c r="B106" s="38"/>
+      <c r="B106" s="37"/>
       <c r="C106" s="28"/>
       <c r="D106" s="29"/>
       <c r="E106" s="29"/>
-      <c r="F106" s="29"/>
+      <c r="F106" s="30"/>
       <c r="G106" s="29"/>
       <c r="H106" s="29"/>
       <c r="I106" s="29"/>
@@ -12866,7 +13118,7 @@
     </row>
     <row r="107" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A107" s="31"/>
-      <c r="B107" s="38"/>
+      <c r="B107" s="37"/>
       <c r="C107" s="28"/>
       <c r="D107" s="29"/>
       <c r="E107" s="29"/>
@@ -12883,11 +13135,11 @@
     </row>
     <row r="108" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A108" s="31"/>
-      <c r="B108" s="38"/>
+      <c r="B108" s="37"/>
       <c r="C108" s="28"/>
       <c r="D108" s="29"/>
       <c r="E108" s="29"/>
-      <c r="F108" s="30"/>
+      <c r="F108" s="29"/>
       <c r="G108" s="29"/>
       <c r="H108" s="29"/>
       <c r="I108" s="29"/>
@@ -12900,10 +13152,10 @@
     </row>
     <row r="109" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A109" s="31"/>
-      <c r="B109" s="38"/>
-      <c r="C109" s="28"/>
-      <c r="D109" s="29"/>
-      <c r="E109" s="29"/>
+      <c r="B109" s="37"/>
+      <c r="C109" s="33"/>
+      <c r="D109" s="30"/>
+      <c r="E109" s="30"/>
       <c r="F109" s="30"/>
       <c r="G109" s="29"/>
       <c r="H109" s="29"/>
@@ -12916,72 +13168,52 @@
       <c r="O109" s="25"/>
     </row>
     <row r="110" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A110" s="31"/>
-      <c r="B110" s="38"/>
+      <c r="A110" s="22"/>
+      <c r="B110" s="23"/>
       <c r="C110" s="28"/>
       <c r="D110" s="29"/>
-      <c r="E110" s="29"/>
+      <c r="E110" s="58"/>
       <c r="F110" s="29"/>
-      <c r="G110" s="29"/>
-      <c r="H110" s="29"/>
-      <c r="I110" s="29"/>
-      <c r="J110" s="48"/>
-      <c r="K110" s="40"/>
-      <c r="L110" s="49"/>
-      <c r="M110" s="50"/>
-      <c r="N110" s="49"/>
+      <c r="G110" s="30"/>
+      <c r="H110" s="30"/>
+      <c r="I110" s="30"/>
+      <c r="J110" s="35"/>
+      <c r="K110" s="25"/>
+      <c r="L110" s="26"/>
+      <c r="M110" s="24"/>
+      <c r="N110" s="26"/>
       <c r="O110" s="25"/>
     </row>
     <row r="111" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A111" s="31"/>
-      <c r="B111" s="38"/>
-      <c r="C111" s="33"/>
-      <c r="D111" s="30"/>
-      <c r="E111" s="30"/>
-      <c r="F111" s="30"/>
-      <c r="G111" s="29"/>
-      <c r="H111" s="29"/>
-      <c r="I111" s="29"/>
-      <c r="J111" s="48"/>
-      <c r="K111" s="40"/>
-      <c r="L111" s="49"/>
-      <c r="M111" s="50"/>
-      <c r="N111" s="49"/>
+      <c r="A111" s="22"/>
+      <c r="B111" s="23"/>
+      <c r="C111" s="28"/>
+      <c r="D111" s="29"/>
+      <c r="E111" s="58"/>
+      <c r="F111" s="32"/>
+      <c r="G111" s="30"/>
+      <c r="H111" s="30"/>
+      <c r="I111" s="30"/>
+      <c r="J111" s="35"/>
+      <c r="K111" s="25"/>
+      <c r="L111" s="26"/>
+      <c r="M111" s="24"/>
+      <c r="N111" s="26"/>
       <c r="O111" s="25"/>
     </row>
-    <row r="112" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A112" s="22"/>
+    <row r="112" ht="19" customHeight="1" spans="2:6">
       <c r="B112" s="23"/>
       <c r="C112" s="28"/>
       <c r="D112" s="29"/>
-      <c r="E112" s="36"/>
-      <c r="F112" s="29"/>
-      <c r="G112" s="30"/>
-      <c r="H112" s="30"/>
-      <c r="I112" s="30"/>
-      <c r="J112" s="35"/>
-      <c r="K112" s="25"/>
-      <c r="L112" s="26"/>
-      <c r="M112" s="24"/>
-      <c r="N112" s="26"/>
-      <c r="O112" s="25"/>
-    </row>
-    <row r="113" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A113" s="22"/>
+      <c r="E112" s="29"/>
+      <c r="F112" s="32"/>
+    </row>
+    <row r="113" ht="19" customHeight="1" spans="2:6">
       <c r="B113" s="23"/>
       <c r="C113" s="28"/>
       <c r="D113" s="29"/>
-      <c r="E113" s="36"/>
+      <c r="E113" s="29"/>
       <c r="F113" s="32"/>
-      <c r="G113" s="30"/>
-      <c r="H113" s="30"/>
-      <c r="I113" s="30"/>
-      <c r="J113" s="35"/>
-      <c r="K113" s="25"/>
-      <c r="L113" s="26"/>
-      <c r="M113" s="24"/>
-      <c r="N113" s="26"/>
-      <c r="O113" s="25"/>
     </row>
     <row r="114" ht="19" customHeight="1" spans="2:6">
       <c r="B114" s="23"/>
@@ -12990,27 +13222,27 @@
       <c r="E114" s="29"/>
       <c r="F114" s="32"/>
     </row>
-    <row r="115" ht="19" customHeight="1" spans="2:6">
+    <row r="115" ht="43" customHeight="1" spans="1:6">
+      <c r="A115" s="22"/>
       <c r="B115" s="23"/>
       <c r="C115" s="28"/>
       <c r="D115" s="29"/>
       <c r="E115" s="29"/>
       <c r="F115" s="32"/>
     </row>
-    <row r="116" ht="19" customHeight="1" spans="2:6">
+    <row r="116" ht="21" customHeight="1" spans="2:6">
       <c r="B116" s="23"/>
       <c r="C116" s="28"/>
       <c r="D116" s="29"/>
       <c r="E116" s="29"/>
       <c r="F116" s="32"/>
     </row>
-    <row r="117" ht="43" customHeight="1" spans="1:6">
-      <c r="A117" s="22"/>
-      <c r="B117" s="23"/>
-      <c r="C117" s="28"/>
-      <c r="D117" s="29"/>
-      <c r="E117" s="29"/>
-      <c r="F117" s="32"/>
+    <row r="117" ht="21" customHeight="1" spans="2:6">
+      <c r="B117" s="59"/>
+      <c r="C117" s="33"/>
+      <c r="D117" s="30"/>
+      <c r="E117" s="30"/>
+      <c r="F117" s="35"/>
     </row>
     <row r="118" ht="21" customHeight="1" spans="2:6">
       <c r="B118" s="23"/>
@@ -13020,51 +13252,71 @@
       <c r="F118" s="32"/>
     </row>
     <row r="119" ht="21" customHeight="1" spans="2:6">
-      <c r="B119" s="59"/>
+      <c r="B119" s="23"/>
       <c r="C119" s="33"/>
       <c r="D119" s="30"/>
       <c r="E119" s="30"/>
-      <c r="F119" s="35"/>
-    </row>
-    <row r="120" ht="21" customHeight="1" spans="2:6">
+      <c r="F119" s="30"/>
+    </row>
+    <row r="120" ht="22" customHeight="1" spans="2:6">
       <c r="B120" s="23"/>
       <c r="C120" s="28"/>
       <c r="D120" s="29"/>
       <c r="E120" s="29"/>
       <c r="F120" s="32"/>
     </row>
-    <row r="121" ht="21" customHeight="1" spans="2:6">
+    <row r="121" customFormat="1" ht="22" customHeight="1" spans="1:15">
+      <c r="A121" s="6"/>
       <c r="B121" s="23"/>
-      <c r="C121" s="33"/>
-      <c r="D121" s="30"/>
-      <c r="E121" s="30"/>
-      <c r="F121" s="30"/>
-    </row>
-    <row r="122" ht="22" customHeight="1" spans="2:6">
+      <c r="C121" s="28"/>
+      <c r="D121" s="29"/>
+      <c r="E121" s="29"/>
+      <c r="F121" s="32"/>
+      <c r="G121" s="9"/>
+      <c r="H121" s="9"/>
+      <c r="I121" s="9"/>
+      <c r="J121" s="10"/>
+      <c r="K121" s="11"/>
+      <c r="L121" s="12"/>
+      <c r="M121" s="13"/>
+      <c r="N121" s="12"/>
+      <c r="O121" s="11"/>
+    </row>
+    <row r="122" customFormat="1" ht="19" customHeight="1" spans="1:15">
+      <c r="A122" s="31"/>
       <c r="B122" s="23"/>
       <c r="C122" s="28"/>
       <c r="D122" s="29"/>
       <c r="E122" s="29"/>
       <c r="F122" s="32"/>
-    </row>
-    <row r="123" customFormat="1" ht="22" customHeight="1" spans="1:15">
-      <c r="A123" s="6"/>
+      <c r="G122" s="29"/>
+      <c r="H122" s="29"/>
+      <c r="I122" s="29"/>
+      <c r="J122" s="48"/>
+      <c r="K122" s="40"/>
+      <c r="L122" s="49"/>
+      <c r="M122" s="50"/>
+      <c r="N122" s="49"/>
+      <c r="O122" s="40"/>
+    </row>
+    <row r="123" customFormat="1" ht="19" customHeight="1" spans="1:15">
+      <c r="A123" s="31"/>
       <c r="B123" s="23"/>
       <c r="C123" s="28"/>
       <c r="D123" s="29"/>
       <c r="E123" s="29"/>
       <c r="F123" s="32"/>
-      <c r="G123" s="9"/>
-      <c r="H123" s="9"/>
-      <c r="I123" s="9"/>
-      <c r="J123" s="10"/>
-      <c r="K123" s="11"/>
-      <c r="L123" s="12"/>
-      <c r="M123" s="13"/>
-      <c r="N123" s="12"/>
-      <c r="O123" s="11"/>
-    </row>
-    <row r="124" customFormat="1" ht="19" customHeight="1" spans="1:15">
+      <c r="G123" s="29"/>
+      <c r="H123" s="29"/>
+      <c r="I123" s="29"/>
+      <c r="J123" s="48"/>
+      <c r="K123" s="40"/>
+      <c r="L123" s="49"/>
+      <c r="M123" s="50"/>
+      <c r="N123" s="49"/>
+      <c r="O123" s="40"/>
+    </row>
+    <row r="124" customFormat="1" ht="29" customHeight="1" spans="1:15">
       <c r="A124" s="31"/>
       <c r="B124" s="23"/>
       <c r="C124" s="28"/>
@@ -13081,7 +13333,7 @@
       <c r="N124" s="49"/>
       <c r="O124" s="40"/>
     </row>
-    <row r="125" customFormat="1" ht="19" customHeight="1" spans="1:15">
+    <row r="125" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A125" s="31"/>
       <c r="B125" s="23"/>
       <c r="C125" s="28"/>
@@ -13098,73 +13350,75 @@
       <c r="N125" s="49"/>
       <c r="O125" s="40"/>
     </row>
-    <row r="126" customFormat="1" ht="29" customHeight="1" spans="1:15">
-      <c r="A126" s="31"/>
+    <row r="126" s="5" customFormat="1" ht="38" customHeight="1" spans="1:15">
+      <c r="A126" s="22"/>
       <c r="B126" s="23"/>
       <c r="C126" s="28"/>
       <c r="D126" s="29"/>
       <c r="E126" s="29"/>
       <c r="F126" s="32"/>
-      <c r="G126" s="29"/>
-      <c r="H126" s="29"/>
-      <c r="I126" s="29"/>
-      <c r="J126" s="48"/>
-      <c r="K126" s="40"/>
-      <c r="L126" s="49"/>
-      <c r="M126" s="50"/>
-      <c r="N126" s="49"/>
-      <c r="O126" s="40"/>
-    </row>
-    <row r="127" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A127" s="31"/>
+      <c r="G126" s="60"/>
+      <c r="H126" s="60"/>
+      <c r="I126" s="60"/>
+      <c r="J126" s="61"/>
+      <c r="K126" s="53"/>
+      <c r="L126" s="51"/>
+      <c r="M126" s="52"/>
+      <c r="N126" s="51"/>
+      <c r="O126" s="53"/>
+    </row>
+    <row r="127" s="5" customFormat="1" ht="25" customHeight="1" spans="1:15">
+      <c r="A127" s="22"/>
       <c r="B127" s="23"/>
       <c r="C127" s="28"/>
       <c r="D127" s="29"/>
       <c r="E127" s="29"/>
       <c r="F127" s="32"/>
-      <c r="G127" s="29"/>
-      <c r="H127" s="29"/>
-      <c r="I127" s="29"/>
-      <c r="J127" s="48"/>
-      <c r="K127" s="40"/>
-      <c r="L127" s="49"/>
-      <c r="M127" s="50"/>
-      <c r="N127" s="49"/>
-      <c r="O127" s="40"/>
-    </row>
-    <row r="128" s="5" customFormat="1" ht="38" customHeight="1" spans="1:15">
-      <c r="A128" s="22"/>
+      <c r="G127" s="60"/>
+      <c r="H127" s="60"/>
+      <c r="I127" s="60"/>
+      <c r="J127" s="61"/>
+      <c r="K127" s="53"/>
+      <c r="L127" s="51"/>
+      <c r="M127" s="52"/>
+      <c r="N127" s="51"/>
+      <c r="O127" s="53"/>
+    </row>
+    <row r="128" s="1" customFormat="1" ht="23" customHeight="1" spans="1:16">
+      <c r="A128" s="31"/>
       <c r="B128" s="23"/>
       <c r="C128" s="28"/>
       <c r="D128" s="29"/>
       <c r="E128" s="29"/>
-      <c r="F128" s="32"/>
-      <c r="G128" s="60"/>
-      <c r="H128" s="60"/>
-      <c r="I128" s="60"/>
-      <c r="J128" s="61"/>
-      <c r="K128" s="53"/>
-      <c r="L128" s="51"/>
-      <c r="M128" s="52"/>
-      <c r="N128" s="51"/>
-      <c r="O128" s="53"/>
-    </row>
-    <row r="129" s="5" customFormat="1" ht="25" customHeight="1" spans="1:15">
-      <c r="A129" s="22"/>
+      <c r="F128" s="29"/>
+      <c r="G128" s="29"/>
+      <c r="H128" s="29"/>
+      <c r="I128" s="29"/>
+      <c r="J128" s="48"/>
+      <c r="K128" s="31"/>
+      <c r="L128" s="23"/>
+      <c r="M128" s="28"/>
+      <c r="N128" s="29"/>
+      <c r="O128" s="29"/>
+      <c r="P128" s="29"/>
+    </row>
+    <row r="129" s="1" customFormat="1" ht="23" customHeight="1" spans="1:16">
+      <c r="A129" s="31"/>
       <c r="B129" s="23"/>
       <c r="C129" s="28"/>
       <c r="D129" s="29"/>
       <c r="E129" s="29"/>
-      <c r="F129" s="32"/>
-      <c r="G129" s="60"/>
-      <c r="H129" s="60"/>
-      <c r="I129" s="60"/>
-      <c r="J129" s="61"/>
-      <c r="K129" s="53"/>
-      <c r="L129" s="51"/>
-      <c r="M129" s="52"/>
-      <c r="N129" s="51"/>
-      <c r="O129" s="53"/>
+      <c r="F129" s="29"/>
+      <c r="G129" s="29"/>
+      <c r="H129" s="29"/>
+      <c r="I129" s="29"/>
+      <c r="J129" s="48"/>
+      <c r="K129" s="31"/>
+      <c r="L129" s="23"/>
+      <c r="M129" s="28"/>
+      <c r="N129" s="29"/>
+      <c r="O129" s="29"/>
+      <c r="P129" s="29"/>
     </row>
     <row r="130" s="1" customFormat="1" ht="23" customHeight="1" spans="1:16">
       <c r="A130" s="31"/>
@@ -13184,7 +13438,7 @@
       <c r="O130" s="29"/>
       <c r="P130" s="29"/>
     </row>
-    <row r="131" s="1" customFormat="1" ht="23" customHeight="1" spans="1:16">
+    <row r="131" customFormat="1" ht="23" customHeight="1" spans="1:16">
       <c r="A131" s="31"/>
       <c r="B131" s="23"/>
       <c r="C131" s="28"/>
@@ -13202,13 +13456,13 @@
       <c r="O131" s="29"/>
       <c r="P131" s="29"/>
     </row>
-    <row r="132" s="1" customFormat="1" ht="23" customHeight="1" spans="1:16">
+    <row r="132" ht="23" customHeight="1" spans="1:16">
       <c r="A132" s="31"/>
       <c r="B132" s="23"/>
       <c r="C132" s="28"/>
       <c r="D132" s="29"/>
       <c r="E132" s="29"/>
-      <c r="F132" s="29"/>
+      <c r="F132" s="32"/>
       <c r="G132" s="29"/>
       <c r="H132" s="29"/>
       <c r="I132" s="29"/>
@@ -13220,13 +13474,13 @@
       <c r="O132" s="29"/>
       <c r="P132" s="29"/>
     </row>
-    <row r="133" customFormat="1" ht="23" customHeight="1" spans="1:16">
+    <row r="133" ht="23" customHeight="1" spans="1:16">
       <c r="A133" s="31"/>
       <c r="B133" s="23"/>
       <c r="C133" s="28"/>
       <c r="D133" s="29"/>
       <c r="E133" s="29"/>
-      <c r="F133" s="29"/>
+      <c r="F133" s="32"/>
       <c r="G133" s="29"/>
       <c r="H133" s="29"/>
       <c r="I133" s="29"/>
@@ -13258,11 +13512,11 @@
     </row>
     <row r="135" ht="23" customHeight="1" spans="1:16">
       <c r="A135" s="31"/>
-      <c r="B135" s="23"/>
-      <c r="C135" s="28"/>
-      <c r="D135" s="29"/>
-      <c r="E135" s="29"/>
-      <c r="F135" s="32"/>
+      <c r="B135" s="37"/>
+      <c r="C135" s="33"/>
+      <c r="D135" s="30"/>
+      <c r="E135" s="30"/>
+      <c r="F135" s="35"/>
       <c r="G135" s="29"/>
       <c r="H135" s="29"/>
       <c r="I135" s="29"/>
@@ -13274,13 +13528,13 @@
       <c r="O135" s="29"/>
       <c r="P135" s="29"/>
     </row>
-    <row r="136" ht="23" customHeight="1" spans="1:16">
+    <row r="136" ht="32" customHeight="1" spans="1:16">
       <c r="A136" s="31"/>
       <c r="B136" s="23"/>
-      <c r="C136" s="28"/>
-      <c r="D136" s="29"/>
-      <c r="E136" s="29"/>
-      <c r="F136" s="32"/>
+      <c r="C136" s="33"/>
+      <c r="D136" s="38"/>
+      <c r="E136" s="30"/>
+      <c r="F136" s="29"/>
       <c r="G136" s="29"/>
       <c r="H136" s="29"/>
       <c r="I136" s="29"/>
@@ -13292,11 +13546,11 @@
       <c r="O136" s="29"/>
       <c r="P136" s="29"/>
     </row>
-    <row r="137" ht="23" customHeight="1" spans="1:16">
+    <row r="137" ht="34" customHeight="1" spans="1:16">
       <c r="A137" s="31"/>
-      <c r="B137" s="38"/>
+      <c r="B137" s="23"/>
       <c r="C137" s="33"/>
-      <c r="D137" s="30"/>
+      <c r="D137" s="38"/>
       <c r="E137" s="30"/>
       <c r="F137" s="35"/>
       <c r="G137" s="29"/>
@@ -13310,13 +13564,13 @@
       <c r="O137" s="29"/>
       <c r="P137" s="29"/>
     </row>
-    <row r="138" ht="32" customHeight="1" spans="1:16">
+    <row r="138" ht="34" customHeight="1" spans="1:16">
       <c r="A138" s="31"/>
       <c r="B138" s="23"/>
-      <c r="C138" s="33"/>
-      <c r="D138" s="62"/>
-      <c r="E138" s="30"/>
-      <c r="F138" s="29"/>
+      <c r="C138" s="28"/>
+      <c r="D138" s="29"/>
+      <c r="E138" s="29"/>
+      <c r="F138" s="32"/>
       <c r="G138" s="29"/>
       <c r="H138" s="29"/>
       <c r="I138" s="29"/>
@@ -13332,9 +13586,9 @@
       <c r="A139" s="31"/>
       <c r="B139" s="23"/>
       <c r="C139" s="33"/>
-      <c r="D139" s="62"/>
-      <c r="E139" s="30"/>
-      <c r="F139" s="35"/>
+      <c r="D139" s="30"/>
+      <c r="E139" s="58"/>
+      <c r="F139" s="32"/>
       <c r="G139" s="29"/>
       <c r="H139" s="29"/>
       <c r="I139" s="29"/>
@@ -13349,10 +13603,10 @@
     <row r="140" ht="34" customHeight="1" spans="1:16">
       <c r="A140" s="31"/>
       <c r="B140" s="23"/>
-      <c r="C140" s="28"/>
-      <c r="D140" s="29"/>
-      <c r="E140" s="29"/>
-      <c r="F140" s="32"/>
+      <c r="C140" s="33"/>
+      <c r="D140" s="30"/>
+      <c r="E140" s="58"/>
+      <c r="F140" s="35"/>
       <c r="G140" s="29"/>
       <c r="H140" s="29"/>
       <c r="I140" s="29"/>
@@ -13369,7 +13623,7 @@
       <c r="B141" s="23"/>
       <c r="C141" s="33"/>
       <c r="D141" s="30"/>
-      <c r="E141" s="36"/>
+      <c r="E141" s="58"/>
       <c r="F141" s="32"/>
       <c r="G141" s="29"/>
       <c r="H141" s="29"/>
@@ -13385,10 +13639,10 @@
     <row r="142" ht="34" customHeight="1" spans="1:16">
       <c r="A142" s="31"/>
       <c r="B142" s="23"/>
-      <c r="C142" s="33"/>
-      <c r="D142" s="30"/>
-      <c r="E142" s="36"/>
-      <c r="F142" s="35"/>
+      <c r="C142" s="28"/>
+      <c r="D142" s="29"/>
+      <c r="E142" s="58"/>
+      <c r="F142" s="32"/>
       <c r="G142" s="29"/>
       <c r="H142" s="29"/>
       <c r="I142" s="29"/>
@@ -13400,13 +13654,13 @@
       <c r="O142" s="29"/>
       <c r="P142" s="29"/>
     </row>
-    <row r="143" ht="34" customHeight="1" spans="1:16">
+    <row r="143" ht="23" customHeight="1" spans="1:16">
       <c r="A143" s="31"/>
       <c r="B143" s="23"/>
-      <c r="C143" s="33"/>
-      <c r="D143" s="30"/>
-      <c r="E143" s="36"/>
-      <c r="F143" s="32"/>
+      <c r="C143" s="28"/>
+      <c r="D143" s="29"/>
+      <c r="E143" s="58"/>
+      <c r="F143" s="29"/>
       <c r="G143" s="29"/>
       <c r="H143" s="29"/>
       <c r="I143" s="29"/>
@@ -13418,12 +13672,12 @@
       <c r="O143" s="29"/>
       <c r="P143" s="29"/>
     </row>
-    <row r="144" ht="34" customHeight="1" spans="1:16">
+    <row r="144" s="1" customFormat="1" ht="23" customHeight="1" spans="1:16">
       <c r="A144" s="31"/>
       <c r="B144" s="23"/>
       <c r="C144" s="28"/>
       <c r="D144" s="29"/>
-      <c r="E144" s="36"/>
+      <c r="E144" s="58"/>
       <c r="F144" s="32"/>
       <c r="G144" s="29"/>
       <c r="H144" s="29"/>
@@ -13436,13 +13690,13 @@
       <c r="O144" s="29"/>
       <c r="P144" s="29"/>
     </row>
-    <row r="145" ht="23" customHeight="1" spans="1:16">
+    <row r="145" s="5" customFormat="1" ht="23" customHeight="1" spans="1:16">
       <c r="A145" s="31"/>
       <c r="B145" s="23"/>
       <c r="C145" s="28"/>
       <c r="D145" s="29"/>
-      <c r="E145" s="36"/>
-      <c r="F145" s="29"/>
+      <c r="E145" s="29"/>
+      <c r="F145" s="32"/>
       <c r="G145" s="29"/>
       <c r="H145" s="29"/>
       <c r="I145" s="29"/>
@@ -13454,12 +13708,12 @@
       <c r="O145" s="29"/>
       <c r="P145" s="29"/>
     </row>
-    <row r="146" s="1" customFormat="1" ht="23" customHeight="1" spans="1:16">
+    <row r="146" s="5" customFormat="1" ht="23" customHeight="1" spans="1:16">
       <c r="A146" s="31"/>
       <c r="B146" s="23"/>
       <c r="C146" s="28"/>
       <c r="D146" s="29"/>
-      <c r="E146" s="36"/>
+      <c r="E146" s="29"/>
       <c r="F146" s="32"/>
       <c r="G146" s="29"/>
       <c r="H146" s="29"/>
@@ -13472,7 +13726,7 @@
       <c r="O146" s="29"/>
       <c r="P146" s="29"/>
     </row>
-    <row r="147" s="5" customFormat="1" ht="23" customHeight="1" spans="1:16">
+    <row r="147" ht="23" customHeight="1" spans="1:16">
       <c r="A147" s="31"/>
       <c r="B147" s="23"/>
       <c r="C147" s="28"/>
@@ -13490,13 +13744,13 @@
       <c r="O147" s="29"/>
       <c r="P147" s="29"/>
     </row>
-    <row r="148" s="5" customFormat="1" ht="23" customHeight="1" spans="1:16">
+    <row r="148" ht="23" customHeight="1" spans="1:16">
       <c r="A148" s="31"/>
       <c r="B148" s="23"/>
       <c r="C148" s="28"/>
       <c r="D148" s="29"/>
       <c r="E148" s="29"/>
-      <c r="F148" s="32"/>
+      <c r="F148" s="29"/>
       <c r="G148" s="29"/>
       <c r="H148" s="29"/>
       <c r="I148" s="29"/>
@@ -13514,7 +13768,7 @@
       <c r="C149" s="28"/>
       <c r="D149" s="29"/>
       <c r="E149" s="29"/>
-      <c r="F149" s="32"/>
+      <c r="F149" s="29"/>
       <c r="G149" s="29"/>
       <c r="H149" s="29"/>
       <c r="I149" s="29"/>
@@ -16010,9 +16264,9 @@
       <c r="O287" s="29"/>
       <c r="P287" s="29"/>
     </row>
-    <row r="288" ht="23" customHeight="1" spans="1:16">
+    <row r="288" ht="23" customHeight="1" spans="1:15">
       <c r="A288" s="31"/>
-      <c r="B288" s="23"/>
+      <c r="B288" s="37"/>
       <c r="C288" s="28"/>
       <c r="D288" s="29"/>
       <c r="E288" s="29"/>
@@ -16021,16 +16275,15 @@
       <c r="H288" s="29"/>
       <c r="I288" s="29"/>
       <c r="J288" s="48"/>
-      <c r="K288" s="31"/>
-      <c r="L288" s="23"/>
-      <c r="M288" s="28"/>
-      <c r="N288" s="29"/>
-      <c r="O288" s="29"/>
-      <c r="P288" s="29"/>
-    </row>
-    <row r="289" ht="23" customHeight="1" spans="1:16">
+      <c r="K288" s="40"/>
+      <c r="L288" s="49"/>
+      <c r="M288" s="50"/>
+      <c r="N288" s="49"/>
+      <c r="O288" s="40"/>
+    </row>
+    <row r="289" ht="23" customHeight="1" spans="1:15">
       <c r="A289" s="31"/>
-      <c r="B289" s="23"/>
+      <c r="B289" s="37"/>
       <c r="C289" s="28"/>
       <c r="D289" s="29"/>
       <c r="E289" s="29"/>
@@ -16039,16 +16292,15 @@
       <c r="H289" s="29"/>
       <c r="I289" s="29"/>
       <c r="J289" s="48"/>
-      <c r="K289" s="31"/>
-      <c r="L289" s="23"/>
-      <c r="M289" s="28"/>
-      <c r="N289" s="29"/>
-      <c r="O289" s="29"/>
-      <c r="P289" s="29"/>
+      <c r="K289" s="40"/>
+      <c r="L289" s="49"/>
+      <c r="M289" s="50"/>
+      <c r="N289" s="49"/>
+      <c r="O289" s="40"/>
     </row>
     <row r="290" ht="23" customHeight="1" spans="1:15">
       <c r="A290" s="31"/>
-      <c r="B290" s="38"/>
+      <c r="B290" s="37"/>
       <c r="C290" s="28"/>
       <c r="D290" s="29"/>
       <c r="E290" s="29"/>
@@ -16065,7 +16317,7 @@
     </row>
     <row r="291" ht="23" customHeight="1" spans="1:15">
       <c r="A291" s="31"/>
-      <c r="B291" s="38"/>
+      <c r="B291" s="37"/>
       <c r="C291" s="28"/>
       <c r="D291" s="29"/>
       <c r="E291" s="29"/>
@@ -16082,7 +16334,7 @@
     </row>
     <row r="292" ht="23" customHeight="1" spans="1:15">
       <c r="A292" s="31"/>
-      <c r="B292" s="38"/>
+      <c r="B292" s="37"/>
       <c r="C292" s="28"/>
       <c r="D292" s="29"/>
       <c r="E292" s="29"/>
@@ -16099,7 +16351,7 @@
     </row>
     <row r="293" ht="23" customHeight="1" spans="1:15">
       <c r="A293" s="31"/>
-      <c r="B293" s="38"/>
+      <c r="B293" s="37"/>
       <c r="C293" s="28"/>
       <c r="D293" s="29"/>
       <c r="E293" s="29"/>
@@ -16116,7 +16368,7 @@
     </row>
     <row r="294" ht="23" customHeight="1" spans="1:15">
       <c r="A294" s="31"/>
-      <c r="B294" s="38"/>
+      <c r="B294" s="37"/>
       <c r="C294" s="28"/>
       <c r="D294" s="29"/>
       <c r="E294" s="29"/>
@@ -16133,7 +16385,7 @@
     </row>
     <row r="295" ht="23" customHeight="1" spans="1:15">
       <c r="A295" s="31"/>
-      <c r="B295" s="38"/>
+      <c r="B295" s="37"/>
       <c r="C295" s="28"/>
       <c r="D295" s="29"/>
       <c r="E295" s="29"/>
@@ -16150,7 +16402,7 @@
     </row>
     <row r="296" ht="23" customHeight="1" spans="1:15">
       <c r="A296" s="31"/>
-      <c r="B296" s="38"/>
+      <c r="B296" s="37"/>
       <c r="C296" s="28"/>
       <c r="D296" s="29"/>
       <c r="E296" s="29"/>
@@ -16167,7 +16419,7 @@
     </row>
     <row r="297" ht="23" customHeight="1" spans="1:15">
       <c r="A297" s="31"/>
-      <c r="B297" s="38"/>
+      <c r="B297" s="37"/>
       <c r="C297" s="28"/>
       <c r="D297" s="29"/>
       <c r="E297" s="29"/>
@@ -16184,7 +16436,7 @@
     </row>
     <row r="298" ht="23" customHeight="1" spans="1:15">
       <c r="A298" s="31"/>
-      <c r="B298" s="38"/>
+      <c r="B298" s="37"/>
       <c r="C298" s="28"/>
       <c r="D298" s="29"/>
       <c r="E298" s="29"/>
@@ -16201,7 +16453,7 @@
     </row>
     <row r="299" ht="23" customHeight="1" spans="1:15">
       <c r="A299" s="31"/>
-      <c r="B299" s="38"/>
+      <c r="B299" s="37"/>
       <c r="C299" s="28"/>
       <c r="D299" s="29"/>
       <c r="E299" s="29"/>
@@ -16218,7 +16470,7 @@
     </row>
     <row r="300" ht="23" customHeight="1" spans="1:15">
       <c r="A300" s="31"/>
-      <c r="B300" s="38"/>
+      <c r="B300" s="37"/>
       <c r="C300" s="28"/>
       <c r="D300" s="29"/>
       <c r="E300" s="29"/>
@@ -16235,7 +16487,7 @@
     </row>
     <row r="301" ht="23" customHeight="1" spans="1:15">
       <c r="A301" s="31"/>
-      <c r="B301" s="38"/>
+      <c r="B301" s="37"/>
       <c r="C301" s="28"/>
       <c r="D301" s="29"/>
       <c r="E301" s="29"/>
@@ -16252,7 +16504,7 @@
     </row>
     <row r="302" ht="23" customHeight="1" spans="1:15">
       <c r="A302" s="31"/>
-      <c r="B302" s="38"/>
+      <c r="B302" s="37"/>
       <c r="C302" s="28"/>
       <c r="D302" s="29"/>
       <c r="E302" s="29"/>
@@ -16269,7 +16521,7 @@
     </row>
     <row r="303" ht="23" customHeight="1" spans="1:15">
       <c r="A303" s="31"/>
-      <c r="B303" s="38"/>
+      <c r="B303" s="37"/>
       <c r="C303" s="28"/>
       <c r="D303" s="29"/>
       <c r="E303" s="29"/>
@@ -16286,7 +16538,7 @@
     </row>
     <row r="304" ht="23" customHeight="1" spans="1:15">
       <c r="A304" s="31"/>
-      <c r="B304" s="38"/>
+      <c r="B304" s="37"/>
       <c r="C304" s="28"/>
       <c r="D304" s="29"/>
       <c r="E304" s="29"/>
@@ -16303,7 +16555,7 @@
     </row>
     <row r="305" ht="23" customHeight="1" spans="1:15">
       <c r="A305" s="31"/>
-      <c r="B305" s="38"/>
+      <c r="B305" s="37"/>
       <c r="C305" s="28"/>
       <c r="D305" s="29"/>
       <c r="E305" s="29"/>
@@ -16320,7 +16572,7 @@
     </row>
     <row r="306" ht="23" customHeight="1" spans="1:15">
       <c r="A306" s="31"/>
-      <c r="B306" s="38"/>
+      <c r="B306" s="37"/>
       <c r="C306" s="28"/>
       <c r="D306" s="29"/>
       <c r="E306" s="29"/>
@@ -16334,40 +16586,6 @@
       <c r="M306" s="50"/>
       <c r="N306" s="49"/>
       <c r="O306" s="40"/>
-    </row>
-    <row r="307" ht="23" customHeight="1" spans="1:15">
-      <c r="A307" s="31"/>
-      <c r="B307" s="38"/>
-      <c r="C307" s="28"/>
-      <c r="D307" s="29"/>
-      <c r="E307" s="29"/>
-      <c r="F307" s="29"/>
-      <c r="G307" s="29"/>
-      <c r="H307" s="29"/>
-      <c r="I307" s="29"/>
-      <c r="J307" s="48"/>
-      <c r="K307" s="40"/>
-      <c r="L307" s="49"/>
-      <c r="M307" s="50"/>
-      <c r="N307" s="49"/>
-      <c r="O307" s="40"/>
-    </row>
-    <row r="308" ht="23" customHeight="1" spans="1:15">
-      <c r="A308" s="31"/>
-      <c r="B308" s="38"/>
-      <c r="C308" s="28"/>
-      <c r="D308" s="29"/>
-      <c r="E308" s="29"/>
-      <c r="F308" s="29"/>
-      <c r="G308" s="29"/>
-      <c r="H308" s="29"/>
-      <c r="I308" s="29"/>
-      <c r="J308" s="48"/>
-      <c r="K308" s="40"/>
-      <c r="L308" s="49"/>
-      <c r="M308" s="50"/>
-      <c r="N308" s="49"/>
-      <c r="O308" s="40"/>
     </row>
   </sheetData>
   <sheetProtection insertRows="0" insertHyperlinks="0" deleteRows="0"/>
@@ -16399,15 +16617,15 @@
       <formula>LEFT(N5,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N42">
+  <conditionalFormatting sqref="N43">
     <cfRule type="beginsWith" dxfId="2" priority="13" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N42,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N43,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="14" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N42,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N43,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="0" priority="15" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N42,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N43,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N4">
@@ -16432,18 +16650,18 @@
       <formula>LEFT(N6,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N43:N45">
+  <conditionalFormatting sqref="N44:N45">
     <cfRule type="beginsWith" dxfId="2" priority="10" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N43,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N44,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="11" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N43,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N44,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="0" priority="12" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N43,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N44,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N46:N50">
+  <conditionalFormatting sqref="N46:N48">
     <cfRule type="beginsWith" dxfId="2" priority="7" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N46,LEN("WARN"))="WARN"</formula>
     </cfRule>
@@ -16454,73 +16672,73 @@
       <formula>LEFT(N46,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N51:N52">
+  <conditionalFormatting sqref="N49:N50">
     <cfRule type="beginsWith" dxfId="2" priority="19" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N51,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N49,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="20" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N51,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N49,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="0" priority="21" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N51,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N49,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N57:N58">
+    <cfRule type="beginsWith" dxfId="2" priority="4" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N57,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="5" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N57,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="6" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N57,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N59:N60">
-    <cfRule type="beginsWith" dxfId="2" priority="4" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N59,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="5" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N59,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="6" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="0" priority="3" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N59,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N61:N62">
-    <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N61,LEN("WARN"))="WARN"</formula>
+  <conditionalFormatting sqref="N123:N125">
+    <cfRule type="beginsWith" dxfId="2" priority="34" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N123,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N61,LEN("FAIL"))="FAIL"</formula>
+    <cfRule type="beginsWith" dxfId="1" priority="35" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N123,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="3" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N61,LEN("PASS"))="PASS"</formula>
+    <cfRule type="beginsWith" dxfId="0" priority="36" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N123,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N125:N127">
-    <cfRule type="beginsWith" dxfId="2" priority="34" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N125,LEN("WARN"))="WARN"</formula>
+  <conditionalFormatting sqref="N126:N127">
+    <cfRule type="beginsWith" dxfId="2" priority="31" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N126,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="35" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N125,LEN("FAIL"))="FAIL"</formula>
+    <cfRule type="beginsWith" dxfId="1" priority="32" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N126,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="36" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N125,LEN("PASS"))="PASS"</formula>
+    <cfRule type="beginsWith" dxfId="0" priority="33" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N126,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N128:N129">
-    <cfRule type="beginsWith" dxfId="2" priority="31" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N128,LEN("WARN"))="WARN"</formula>
+  <conditionalFormatting sqref="N288:N306">
+    <cfRule type="beginsWith" dxfId="2" priority="58" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N288,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="32" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N128,LEN("FAIL"))="FAIL"</formula>
+    <cfRule type="beginsWith" dxfId="1" priority="59" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N288,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="33" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N128,LEN("PASS"))="PASS"</formula>
+    <cfRule type="beginsWith" dxfId="0" priority="60" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N288,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N290:N308">
-    <cfRule type="beginsWith" dxfId="2" priority="58" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N290,LEN("WARN"))="WARN"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="59" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N290,LEN("FAIL"))="FAIL"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="60" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N290,LEN("PASS"))="PASS"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N35:N40 N112:N113">
+  <conditionalFormatting sqref="N35:N40 N110:N111">
     <cfRule type="beginsWith" dxfId="2" priority="46" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N35,LEN("WARN"))="WARN"</formula>
     </cfRule>
@@ -16531,22 +16749,22 @@
       <formula>LEFT(N35,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N53:N58 N63:N111">
+  <conditionalFormatting sqref="N51:N56 N61:N109">
     <cfRule type="beginsWith" dxfId="2" priority="16" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N53,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N51,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="17" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N53,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N51,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="0" priority="18" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N53,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N51,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C7 C8 C9 C10 C11 C12 C13 C14 C15 C16 C17 C18 C19 C20 C21 C26 C29 C30 C31 C32 C33 C34 C35 C36 C37 C38 C39 C40 C41 C42 C43 C44 C45 C46 C47 C48 C49 C50 C51 C52 C55 C56 C57 C58 C59 C60 C61 C62 C63 C64 C65 C66 C67 C68 C69 C70 C71 C72 C75 C76 C77 C78 C79 C80 C81 C82 C83 C84 C85 C86 C87 C90 C93 C94 C95 C98 C99 C100 C101 C104 C105 C106 C107 C110 C111 C112 C113 C119 C120 C121 C124 C125 C136 C139 C140 C141 C142 C143 C144 C145 C146 C22:C25 C27:C28 C53:C54 C73:C74 C88:C89 C91:C92 C96:C97 C102:C103 C108:C109 C114:C116 C117:C118 C122:C123 C126:C127 C128:C129 C130:C133 C134:C135 C137:C138 C147:C149 C150:C203 C204:C245 C246:C308">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C7 C8 C9 C10 C11 C12 C13 C14 C15 C16 C17 C18 C19 C20 C21 C26 C29 C30 C31 C32 C33 C34 C35 C36 C37 C38 C39 C40 C41 C42 C43 C44 C45 C46 C47 C48 C51 C52 C53 C54 C55 C56 C57 C58 C59 C60 C61 C62 C63 C64 C65 C66 C67 C68 C69 C70 C73 C74 C75 C76 C77 C78 C79 C80 C81 C82 C83 C84 C85 C88 C91 C92 C93 C96 C97 C98 C99 C102 C103 C104 C105 C108 C109 C110 C111 C117 C118 C119 C122 C123 C134 C137 C138 C139 C140 C141 C142 C143 C144 C22:C25 C27:C28 C49:C50 C71:C72 C86:C87 C89:C90 C94:C95 C100:C101 C106:C107 C112:C114 C115:C116 C120:C121 C124:C125 C126:C127 C128:C131 C132:C133 C135:C136 C145:C147 C148:C201 C202:C243 C244:C306">
       <formula1>target</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D26 D29 D30 D31 D32 D33 D34 D35 D36 D37 D38 D39 D40 D41 D42 D43 D44 D45 D46 D47 D48 D49 D50 D51 D52 D55 D56 D57 D58 D59 D60 D61 D62 D63 D64 D65 D66 D67 D68 D69 D70 D71 D72 D75 D76 D77 D78 D79 D80 D81 D82 D83 D84 D85 D86 D87 D90 D91 D92 D93 D94 D95 D98 D99 D100 D101 D104 D105 D106 D107 D110 D111 D112 D113 D119 D120 D121 D124 D125 D136 D139 D140 D141 D142 D143 D144 D145 D146 D6:D7 D22:D25 D27:D28 D53:D54 D73:D74 D88:D89 D96:D97 D102:D103 D108:D109 D114:D116 D117:D118 D122:D123 D126:D127 D128:D129 D130:D133 D134:D135 D137:D138 D147:D149 D150:D192 D193:D308">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D26 D29 D30 D31 D32 D33 D34 D35 D36 D37 D38 D39 D40 D41 D42 D43 D44 D45 D46 D47 D48 D51 D52 D53 D54 D55 D56 D57 D58 D59 D60 D61 D62 D63 D64 D65 D66 D67 D68 D69 D70 D73 D74 D75 D76 D77 D78 D79 D80 D81 D82 D83 D84 D85 D88 D89 D90 D91 D92 D93 D96 D97 D98 D99 D102 D103 D104 D105 D108 D109 D110 D111 D117 D118 D119 D122 D123 D134 D137 D138 D139 D140 D141 D142 D143 D144 D6:D7 D22:D25 D27:D28 D49:D50 D71:D72 D86:D87 D94:D95 D100:D101 D106:D107 D112:D114 D115:D116 D120:D121 D124:D125 D126:D127 D128:D131 D132:D133 D135:D136 D145:D147 D148:D190 D191:D306">
       <formula1>INDIRECT(C5)</formula1>
     </dataValidation>
   </dataValidations>
@@ -16560,10 +16778,10 @@
   <sheetPr/>
   <dimension ref="A1:P275"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
@@ -16751,7 +16969,7 @@
     </row>
     <row r="7" s="4" customFormat="1" ht="29" customHeight="1" spans="1:15">
       <c r="A7" s="31" t="s">
-        <v>838</v>
+        <v>875</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>760</v>
@@ -17048,7 +17266,7 @@
         <v>576</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>839</v>
+        <v>876</v>
       </c>
       <c r="F18" s="32" t="s">
         <v>752</v>
@@ -17580,7 +17798,7 @@
     </row>
     <row r="38" ht="34" customHeight="1" spans="1:16">
       <c r="A38" s="22" t="s">
-        <v>840</v>
+        <v>877</v>
       </c>
       <c r="B38" s="23" t="s">
         <v>835</v>
@@ -17638,15 +17856,25 @@
     </row>
     <row r="40" ht="34" customHeight="1" spans="1:16">
       <c r="A40" s="31"/>
-      <c r="B40" s="23"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="48"/>
+      <c r="B40" s="23" t="s">
+        <v>838</v>
+      </c>
+      <c r="C40" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" s="29" t="s">
+        <v>530</v>
+      </c>
+      <c r="E40" s="34" t="s">
+        <v>839</v>
+      </c>
+      <c r="F40" s="32" t="s">
+        <v>840</v>
+      </c>
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="35"/>
       <c r="K40" s="31"/>
       <c r="L40" s="23"/>
       <c r="M40" s="28"/>
@@ -17656,11 +17884,21 @@
     </row>
     <row r="41" ht="34" customHeight="1" spans="1:16">
       <c r="A41" s="22"/>
-      <c r="B41" s="23"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="37"/>
+      <c r="B41" s="23" t="s">
+        <v>841</v>
+      </c>
+      <c r="C41" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" s="30" t="s">
+        <v>530</v>
+      </c>
+      <c r="E41" s="29" t="s">
+        <v>842</v>
+      </c>
+      <c r="F41" s="36" t="s">
+        <v>843</v>
+      </c>
       <c r="G41" s="29"/>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
@@ -17674,11 +17912,21 @@
     </row>
     <row r="42" ht="34" customHeight="1" spans="1:16">
       <c r="A42" s="22"/>
-      <c r="B42" s="23"/>
-      <c r="C42" s="33"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="32"/>
+      <c r="B42" s="23" t="s">
+        <v>844</v>
+      </c>
+      <c r="C42" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" s="30" t="s">
+        <v>493</v>
+      </c>
+      <c r="E42" s="29" t="s">
+        <v>845</v>
+      </c>
+      <c r="F42" s="29" t="s">
+        <v>846</v>
+      </c>
       <c r="G42" s="29"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
@@ -17692,15 +17940,25 @@
     </row>
     <row r="43" ht="34" customHeight="1" spans="1:16">
       <c r="A43" s="22"/>
-      <c r="B43" s="23"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
+      <c r="B43" s="23" t="s">
+        <v>847</v>
+      </c>
+      <c r="C43" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43" s="29" t="s">
+        <v>530</v>
+      </c>
+      <c r="E43" s="29" t="s">
+        <v>846</v>
+      </c>
+      <c r="F43" s="32" t="s">
+        <v>848</v>
+      </c>
       <c r="G43" s="29"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="35"/>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
@@ -17710,11 +17968,21 @@
     </row>
     <row r="44" ht="34" customHeight="1" spans="1:16">
       <c r="A44" s="31"/>
-      <c r="B44" s="23"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
+      <c r="B44" s="23" t="s">
+        <v>849</v>
+      </c>
+      <c r="C44" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" s="29" t="s">
+        <v>576</v>
+      </c>
+      <c r="E44" s="29" t="s">
+        <v>850</v>
+      </c>
+      <c r="F44" s="29" t="s">
+        <v>752</v>
+      </c>
       <c r="G44" s="29"/>
       <c r="H44" s="29"/>
       <c r="I44" s="29"/>
@@ -17728,11 +17996,21 @@
     </row>
     <row r="45" ht="34" customHeight="1" spans="1:16">
       <c r="A45" s="31"/>
-      <c r="B45" s="38"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
+      <c r="B45" s="23" t="s">
+        <v>851</v>
+      </c>
+      <c r="C45" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="29" t="s">
+        <v>576</v>
+      </c>
+      <c r="E45" s="29" t="s">
+        <v>852</v>
+      </c>
+      <c r="F45" s="29" t="s">
+        <v>752</v>
+      </c>
       <c r="G45" s="29"/>
       <c r="H45" s="29"/>
       <c r="I45" s="29"/>
@@ -17746,11 +18024,21 @@
     </row>
     <row r="46" ht="34" customHeight="1" spans="1:16">
       <c r="A46" s="22"/>
-      <c r="B46" s="38"/>
-      <c r="C46" s="33"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="30"/>
-      <c r="F46" s="30"/>
+      <c r="B46" s="23" t="s">
+        <v>853</v>
+      </c>
+      <c r="C46" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" s="29" t="s">
+        <v>483</v>
+      </c>
+      <c r="E46" s="29" t="s">
+        <v>854</v>
+      </c>
+      <c r="F46" s="30" t="s">
+        <v>855</v>
+      </c>
       <c r="G46" s="29"/>
       <c r="H46" s="30"/>
       <c r="I46" s="30"/>
@@ -17764,11 +18052,21 @@
     </row>
     <row r="47" ht="34" customHeight="1" spans="1:16">
       <c r="A47" s="22"/>
-      <c r="B47" s="23"/>
-      <c r="C47" s="33"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="30"/>
+      <c r="B47" s="23" t="s">
+        <v>856</v>
+      </c>
+      <c r="C47" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" s="29" t="s">
+        <v>493</v>
+      </c>
+      <c r="E47" s="29" t="s">
+        <v>857</v>
+      </c>
+      <c r="F47" s="30" t="s">
+        <v>855</v>
+      </c>
       <c r="G47" s="29"/>
       <c r="H47" s="30"/>
       <c r="I47" s="30"/>
@@ -17782,11 +18080,21 @@
     </row>
     <row r="48" ht="34" customHeight="1" spans="1:16">
       <c r="A48" s="22"/>
-      <c r="B48" s="23"/>
-      <c r="C48" s="33"/>
-      <c r="D48" s="30"/>
-      <c r="E48" s="30"/>
-      <c r="F48" s="30"/>
+      <c r="B48" s="23" t="s">
+        <v>858</v>
+      </c>
+      <c r="C48" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="29" t="s">
+        <v>471</v>
+      </c>
+      <c r="E48" s="29" t="s">
+        <v>859</v>
+      </c>
+      <c r="F48" s="30" t="s">
+        <v>860</v>
+      </c>
       <c r="G48" s="29"/>
       <c r="H48" s="30"/>
       <c r="I48" s="30"/>
@@ -17800,15 +18108,25 @@
     </row>
     <row r="49" ht="34" customHeight="1" spans="1:16">
       <c r="A49" s="22"/>
-      <c r="B49" s="23"/>
-      <c r="C49" s="33"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="30"/>
+      <c r="B49" s="23" t="s">
+        <v>861</v>
+      </c>
+      <c r="C49" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="30" t="s">
+        <v>465</v>
+      </c>
+      <c r="E49" s="30" t="s">
+        <v>862</v>
+      </c>
+      <c r="F49" s="35" t="s">
+        <v>863</v>
+      </c>
       <c r="G49" s="29"/>
-      <c r="H49" s="30"/>
-      <c r="I49" s="30"/>
-      <c r="J49" s="35"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="29"/>
+      <c r="J49" s="48"/>
       <c r="K49" s="25"/>
       <c r="L49" s="26"/>
       <c r="M49" s="24"/>
@@ -17818,15 +18136,25 @@
     </row>
     <row r="50" ht="34" customHeight="1" spans="1:16">
       <c r="A50" s="22"/>
-      <c r="B50" s="23"/>
-      <c r="C50" s="33"/>
-      <c r="D50" s="30"/>
-      <c r="E50" s="30"/>
-      <c r="F50" s="30"/>
+      <c r="B50" s="37" t="s">
+        <v>864</v>
+      </c>
+      <c r="C50" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="E50" s="30" t="s">
+        <v>865</v>
+      </c>
+      <c r="F50" s="29" t="s">
+        <v>866</v>
+      </c>
       <c r="G50" s="29"/>
-      <c r="H50" s="30"/>
-      <c r="I50" s="30"/>
-      <c r="J50" s="35"/>
+      <c r="H50" s="29"/>
+      <c r="I50" s="29"/>
+      <c r="J50" s="48"/>
       <c r="K50" s="25"/>
       <c r="L50" s="26"/>
       <c r="M50" s="24"/>
@@ -17836,11 +18164,21 @@
     </row>
     <row r="51" ht="34" customHeight="1" spans="1:16">
       <c r="A51" s="31"/>
-      <c r="B51" s="23"/>
-      <c r="C51" s="33"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="30"/>
-      <c r="F51" s="30"/>
+      <c r="B51" s="37" t="s">
+        <v>867</v>
+      </c>
+      <c r="C51" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D51" s="38" t="s">
+        <v>302</v>
+      </c>
+      <c r="E51" s="30" t="s">
+        <v>859</v>
+      </c>
+      <c r="F51" s="35" t="s">
+        <v>868</v>
+      </c>
       <c r="G51" s="29"/>
       <c r="H51" s="29"/>
       <c r="I51" s="29"/>
@@ -17854,11 +18192,21 @@
     </row>
     <row r="52" ht="34" customHeight="1" spans="1:16">
       <c r="A52" s="31"/>
-      <c r="B52" s="38"/>
-      <c r="C52" s="28"/>
-      <c r="D52" s="29"/>
-      <c r="E52" s="29"/>
-      <c r="F52" s="29"/>
+      <c r="B52" s="37" t="s">
+        <v>869</v>
+      </c>
+      <c r="C52" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52" s="29" t="s">
+        <v>493</v>
+      </c>
+      <c r="E52" s="29" t="s">
+        <v>870</v>
+      </c>
+      <c r="F52" s="32" t="s">
+        <v>871</v>
+      </c>
       <c r="G52" s="29"/>
       <c r="H52" s="29"/>
       <c r="I52" s="29"/>
@@ -17872,15 +18220,27 @@
     </row>
     <row r="53" ht="34" customHeight="1" spans="1:16">
       <c r="A53" s="31"/>
-      <c r="B53" s="38"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="29"/>
-      <c r="F53" s="29"/>
+      <c r="B53" s="37" t="s">
+        <v>872</v>
+      </c>
+      <c r="C53" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="E53" s="29" t="s">
+        <v>873</v>
+      </c>
+      <c r="F53" s="32" t="s">
+        <v>848</v>
+      </c>
       <c r="G53" s="29"/>
       <c r="H53" s="29"/>
       <c r="I53" s="29"/>
-      <c r="J53" s="48"/>
+      <c r="J53" s="48" t="s">
+        <v>874</v>
+      </c>
       <c r="K53" s="40"/>
       <c r="L53" s="49"/>
       <c r="M53" s="50"/>
@@ -17890,7 +18250,7 @@
     </row>
     <row r="54" ht="34" customHeight="1" spans="1:16">
       <c r="A54" s="31"/>
-      <c r="B54" s="38"/>
+      <c r="B54" s="37"/>
       <c r="C54" s="28"/>
       <c r="D54" s="29"/>
       <c r="E54" s="29"/>
@@ -17908,7 +18268,7 @@
     </row>
     <row r="55" ht="34" customHeight="1" spans="1:16">
       <c r="A55" s="31"/>
-      <c r="B55" s="38"/>
+      <c r="B55" s="37"/>
       <c r="C55" s="28"/>
       <c r="D55" s="29"/>
       <c r="E55" s="29"/>
@@ -17926,7 +18286,7 @@
     </row>
     <row r="56" ht="34" customHeight="1" spans="1:16">
       <c r="A56" s="31"/>
-      <c r="B56" s="38"/>
+      <c r="B56" s="37"/>
       <c r="C56" s="33"/>
       <c r="D56" s="30"/>
       <c r="E56" s="30"/>
@@ -17944,7 +18304,7 @@
     </row>
     <row r="57" ht="34" customHeight="1" spans="1:16">
       <c r="A57" s="31"/>
-      <c r="B57" s="38"/>
+      <c r="B57" s="37"/>
       <c r="C57" s="28"/>
       <c r="D57" s="29"/>
       <c r="E57" s="29"/>
@@ -17962,7 +18322,7 @@
     </row>
     <row r="58" ht="34" customHeight="1" spans="1:16">
       <c r="A58" s="31"/>
-      <c r="B58" s="38"/>
+      <c r="B58" s="37"/>
       <c r="C58" s="33"/>
       <c r="D58" s="30"/>
       <c r="E58" s="30"/>
@@ -17980,7 +18340,7 @@
     </row>
     <row r="59" ht="34" customHeight="1" spans="1:16">
       <c r="A59" s="31"/>
-      <c r="B59" s="38"/>
+      <c r="B59" s="37"/>
       <c r="C59" s="28"/>
       <c r="D59" s="29"/>
       <c r="E59" s="29"/>
@@ -17998,7 +18358,7 @@
     </row>
     <row r="60" ht="34" customHeight="1" spans="1:16">
       <c r="A60" s="31"/>
-      <c r="B60" s="38"/>
+      <c r="B60" s="37"/>
       <c r="C60" s="33"/>
       <c r="D60" s="30"/>
       <c r="E60" s="30"/>
@@ -18016,7 +18376,7 @@
     </row>
     <row r="61" ht="34" customHeight="1" spans="1:16">
       <c r="A61" s="31"/>
-      <c r="B61" s="38"/>
+      <c r="B61" s="37"/>
       <c r="C61" s="28"/>
       <c r="D61" s="29"/>
       <c r="E61" s="29"/>
@@ -18034,7 +18394,7 @@
     </row>
     <row r="62" ht="34" customHeight="1" spans="1:16">
       <c r="A62" s="31"/>
-      <c r="B62" s="38"/>
+      <c r="B62" s="37"/>
       <c r="C62" s="33"/>
       <c r="D62" s="30"/>
       <c r="E62" s="30"/>
@@ -18052,7 +18412,7 @@
     </row>
     <row r="63" ht="34" customHeight="1" spans="1:16">
       <c r="A63" s="31"/>
-      <c r="B63" s="38"/>
+      <c r="B63" s="37"/>
       <c r="C63" s="33"/>
       <c r="D63" s="30"/>
       <c r="E63" s="29"/>
@@ -18070,7 +18430,7 @@
     </row>
     <row r="64" ht="34" customHeight="1" spans="1:16">
       <c r="A64" s="31"/>
-      <c r="B64" s="38"/>
+      <c r="B64" s="37"/>
       <c r="C64" s="28"/>
       <c r="D64" s="29"/>
       <c r="E64" s="29"/>
@@ -18088,7 +18448,7 @@
     </row>
     <row r="65" ht="34" customHeight="1" spans="1:16">
       <c r="A65" s="31"/>
-      <c r="B65" s="38"/>
+      <c r="B65" s="37"/>
       <c r="C65" s="28"/>
       <c r="D65" s="29"/>
       <c r="E65" s="29"/>
@@ -18106,7 +18466,7 @@
     </row>
     <row r="66" ht="34" customHeight="1" spans="1:16">
       <c r="A66" s="31"/>
-      <c r="B66" s="38"/>
+      <c r="B66" s="37"/>
       <c r="C66" s="28"/>
       <c r="D66" s="29"/>
       <c r="E66" s="29"/>
@@ -18124,7 +18484,7 @@
     </row>
     <row r="67" ht="34" customHeight="1" spans="1:16">
       <c r="A67" s="31"/>
-      <c r="B67" s="38"/>
+      <c r="B67" s="37"/>
       <c r="C67" s="33"/>
       <c r="D67" s="30"/>
       <c r="E67" s="30"/>
@@ -18142,7 +18502,7 @@
     </row>
     <row r="68" ht="34" customHeight="1" spans="1:16">
       <c r="A68" s="31"/>
-      <c r="B68" s="38"/>
+      <c r="B68" s="37"/>
       <c r="C68" s="28"/>
       <c r="D68" s="29"/>
       <c r="E68" s="29"/>
@@ -18160,7 +18520,7 @@
     </row>
     <row r="69" ht="34" customHeight="1" spans="1:16">
       <c r="A69" s="31"/>
-      <c r="B69" s="38"/>
+      <c r="B69" s="37"/>
       <c r="C69" s="28"/>
       <c r="D69" s="29"/>
       <c r="E69" s="29"/>
@@ -18178,7 +18538,7 @@
     </row>
     <row r="70" ht="34" customHeight="1" spans="1:16">
       <c r="A70" s="31"/>
-      <c r="B70" s="38"/>
+      <c r="B70" s="37"/>
       <c r="C70" s="28"/>
       <c r="D70" s="29"/>
       <c r="E70" s="29"/>
@@ -18196,7 +18556,7 @@
     </row>
     <row r="71" ht="34" customHeight="1" spans="1:16">
       <c r="A71" s="31"/>
-      <c r="B71" s="38"/>
+      <c r="B71" s="37"/>
       <c r="C71" s="33"/>
       <c r="D71" s="30"/>
       <c r="E71" s="30"/>
@@ -18214,7 +18574,7 @@
     </row>
     <row r="72" ht="34" customHeight="1" spans="1:16">
       <c r="A72" s="31"/>
-      <c r="B72" s="38"/>
+      <c r="B72" s="37"/>
       <c r="C72" s="28"/>
       <c r="D72" s="29"/>
       <c r="E72" s="29"/>
@@ -18232,7 +18592,7 @@
     </row>
     <row r="73" ht="34" customHeight="1" spans="1:16">
       <c r="A73" s="31"/>
-      <c r="B73" s="38"/>
+      <c r="B73" s="37"/>
       <c r="C73" s="28"/>
       <c r="D73" s="29"/>
       <c r="E73" s="29"/>
@@ -18250,7 +18610,7 @@
     </row>
     <row r="74" ht="34" customHeight="1" spans="1:16">
       <c r="A74" s="31"/>
-      <c r="B74" s="38"/>
+      <c r="B74" s="37"/>
       <c r="C74" s="28"/>
       <c r="D74" s="29"/>
       <c r="E74" s="29"/>
@@ -18268,7 +18628,7 @@
     </row>
     <row r="75" ht="34" customHeight="1" spans="1:16">
       <c r="A75" s="31"/>
-      <c r="B75" s="38"/>
+      <c r="B75" s="37"/>
       <c r="C75" s="28"/>
       <c r="D75" s="29"/>
       <c r="E75" s="29"/>
@@ -18286,7 +18646,7 @@
     </row>
     <row r="76" ht="34" customHeight="1" spans="1:16">
       <c r="A76" s="31"/>
-      <c r="B76" s="38"/>
+      <c r="B76" s="37"/>
       <c r="C76" s="33"/>
       <c r="D76" s="30"/>
       <c r="E76" s="30"/>
@@ -18304,7 +18664,7 @@
     </row>
     <row r="77" ht="34" customHeight="1" spans="1:16">
       <c r="A77" s="31"/>
-      <c r="B77" s="38"/>
+      <c r="B77" s="37"/>
       <c r="C77" s="28"/>
       <c r="D77" s="29"/>
       <c r="E77" s="29"/>
@@ -18322,7 +18682,7 @@
     </row>
     <row r="78" ht="34" customHeight="1" spans="1:16">
       <c r="A78" s="31"/>
-      <c r="B78" s="38"/>
+      <c r="B78" s="37"/>
       <c r="C78" s="33"/>
       <c r="D78" s="30"/>
       <c r="E78" s="30"/>
@@ -18340,7 +18700,7 @@
     </row>
     <row r="79" ht="34" customHeight="1" spans="1:16">
       <c r="A79" s="31"/>
-      <c r="B79" s="38"/>
+      <c r="B79" s="37"/>
       <c r="C79" s="28"/>
       <c r="D79" s="29"/>
       <c r="E79" s="29"/>
@@ -18358,7 +18718,7 @@
     </row>
     <row r="80" ht="34" customHeight="1" spans="1:16">
       <c r="A80" s="31"/>
-      <c r="B80" s="38"/>
+      <c r="B80" s="37"/>
       <c r="C80" s="33"/>
       <c r="D80" s="30"/>
       <c r="E80" s="30"/>
@@ -18376,7 +18736,7 @@
     </row>
     <row r="81" ht="34" customHeight="1" spans="1:16">
       <c r="A81" s="31"/>
-      <c r="B81" s="38"/>
+      <c r="B81" s="37"/>
       <c r="C81" s="33"/>
       <c r="D81" s="30"/>
       <c r="E81" s="29"/>
@@ -18394,7 +18754,7 @@
     </row>
     <row r="82" ht="34" customHeight="1" spans="1:16">
       <c r="A82" s="31"/>
-      <c r="B82" s="38"/>
+      <c r="B82" s="37"/>
       <c r="C82" s="28"/>
       <c r="D82" s="29"/>
       <c r="E82" s="29"/>
@@ -18412,7 +18772,7 @@
     </row>
     <row r="83" ht="34" customHeight="1" spans="1:16">
       <c r="A83" s="31"/>
-      <c r="B83" s="38"/>
+      <c r="B83" s="37"/>
       <c r="C83" s="28"/>
       <c r="D83" s="29"/>
       <c r="E83" s="29"/>
@@ -18430,7 +18790,7 @@
     </row>
     <row r="84" ht="34" customHeight="1" spans="1:16">
       <c r="A84" s="31"/>
-      <c r="B84" s="38"/>
+      <c r="B84" s="37"/>
       <c r="C84" s="28"/>
       <c r="D84" s="29"/>
       <c r="E84" s="29"/>
@@ -18448,7 +18808,7 @@
     </row>
     <row r="85" ht="34" customHeight="1" spans="1:16">
       <c r="A85" s="31"/>
-      <c r="B85" s="38"/>
+      <c r="B85" s="37"/>
       <c r="C85" s="28"/>
       <c r="D85" s="29"/>
       <c r="E85" s="29"/>
@@ -18466,7 +18826,7 @@
     </row>
     <row r="86" ht="34" customHeight="1" spans="1:16">
       <c r="A86" s="31"/>
-      <c r="B86" s="38"/>
+      <c r="B86" s="37"/>
       <c r="C86" s="28"/>
       <c r="D86" s="29"/>
       <c r="E86" s="29"/>
@@ -18484,7 +18844,7 @@
     </row>
     <row r="87" ht="34" customHeight="1" spans="1:16">
       <c r="A87" s="31"/>
-      <c r="B87" s="38"/>
+      <c r="B87" s="37"/>
       <c r="C87" s="28"/>
       <c r="D87" s="29"/>
       <c r="E87" s="29"/>
@@ -18502,7 +18862,7 @@
     </row>
     <row r="88" ht="34" customHeight="1" spans="1:16">
       <c r="A88" s="31"/>
-      <c r="B88" s="38"/>
+      <c r="B88" s="37"/>
       <c r="C88" s="28"/>
       <c r="D88" s="29"/>
       <c r="E88" s="29"/>
@@ -18520,7 +18880,7 @@
     </row>
     <row r="89" ht="34" customHeight="1" spans="1:16">
       <c r="A89" s="31"/>
-      <c r="B89" s="38"/>
+      <c r="B89" s="37"/>
       <c r="C89" s="28"/>
       <c r="D89" s="29"/>
       <c r="E89" s="29"/>
@@ -18538,7 +18898,7 @@
     </row>
     <row r="90" ht="34" customHeight="1" spans="1:16">
       <c r="A90" s="31"/>
-      <c r="B90" s="38"/>
+      <c r="B90" s="37"/>
       <c r="C90" s="28"/>
       <c r="D90" s="29"/>
       <c r="E90" s="29"/>
@@ -18556,7 +18916,7 @@
     </row>
     <row r="91" ht="34" customHeight="1" spans="1:16">
       <c r="A91" s="31"/>
-      <c r="B91" s="38"/>
+      <c r="B91" s="37"/>
       <c r="C91" s="28"/>
       <c r="D91" s="29"/>
       <c r="E91" s="29"/>
@@ -18574,7 +18934,7 @@
     </row>
     <row r="92" ht="34" customHeight="1" spans="1:16">
       <c r="A92" s="31"/>
-      <c r="B92" s="38"/>
+      <c r="B92" s="37"/>
       <c r="C92" s="28"/>
       <c r="D92" s="29"/>
       <c r="E92" s="29"/>
@@ -18592,7 +18952,7 @@
     </row>
     <row r="93" ht="34" customHeight="1" spans="1:16">
       <c r="A93" s="31"/>
-      <c r="B93" s="38"/>
+      <c r="B93" s="37"/>
       <c r="C93" s="28"/>
       <c r="D93" s="29"/>
       <c r="E93" s="29"/>
@@ -18610,7 +18970,7 @@
     </row>
     <row r="94" ht="34" customHeight="1" spans="1:16">
       <c r="A94" s="31"/>
-      <c r="B94" s="38"/>
+      <c r="B94" s="37"/>
       <c r="C94" s="28"/>
       <c r="D94" s="29"/>
       <c r="E94" s="29"/>
@@ -18628,7 +18988,7 @@
     </row>
     <row r="95" ht="34" customHeight="1" spans="1:16">
       <c r="A95" s="31"/>
-      <c r="B95" s="38"/>
+      <c r="B95" s="37"/>
       <c r="C95" s="28"/>
       <c r="D95" s="29"/>
       <c r="E95" s="29"/>
@@ -18646,7 +19006,7 @@
     </row>
     <row r="96" ht="34" customHeight="1" spans="1:16">
       <c r="A96" s="31"/>
-      <c r="B96" s="38"/>
+      <c r="B96" s="37"/>
       <c r="C96" s="28"/>
       <c r="D96" s="29"/>
       <c r="E96" s="29"/>
@@ -18664,7 +19024,7 @@
     </row>
     <row r="97" ht="34" customHeight="1" spans="1:16">
       <c r="A97" s="31"/>
-      <c r="B97" s="38"/>
+      <c r="B97" s="37"/>
       <c r="C97" s="28"/>
       <c r="D97" s="29"/>
       <c r="E97" s="29"/>
@@ -18682,7 +19042,7 @@
     </row>
     <row r="98" ht="34" customHeight="1" spans="1:16">
       <c r="A98" s="31"/>
-      <c r="B98" s="38"/>
+      <c r="B98" s="37"/>
       <c r="C98" s="28"/>
       <c r="D98" s="29"/>
       <c r="E98" s="29"/>
@@ -18700,7 +19060,7 @@
     </row>
     <row r="99" ht="34" customHeight="1" spans="1:16">
       <c r="A99" s="31"/>
-      <c r="B99" s="38"/>
+      <c r="B99" s="37"/>
       <c r="C99" s="33"/>
       <c r="D99" s="30"/>
       <c r="E99" s="30"/>
@@ -18718,7 +19078,7 @@
     </row>
     <row r="100" ht="34" customHeight="1" spans="1:16">
       <c r="A100" s="31"/>
-      <c r="B100" s="38"/>
+      <c r="B100" s="37"/>
       <c r="C100" s="33"/>
       <c r="D100" s="30"/>
       <c r="E100" s="29"/>
@@ -18736,7 +19096,7 @@
     </row>
     <row r="101" ht="34" customHeight="1" spans="1:16">
       <c r="A101" s="31"/>
-      <c r="B101" s="38"/>
+      <c r="B101" s="37"/>
       <c r="C101" s="28"/>
       <c r="D101" s="29"/>
       <c r="E101" s="29"/>
@@ -18754,7 +19114,7 @@
     </row>
     <row r="102" ht="34" customHeight="1" spans="1:15">
       <c r="A102" s="31"/>
-      <c r="B102" s="38"/>
+      <c r="B102" s="37"/>
       <c r="C102" s="28"/>
       <c r="D102" s="29"/>
       <c r="E102" s="29"/>
@@ -18771,7 +19131,7 @@
     </row>
     <row r="103" ht="34" customHeight="1" spans="1:15">
       <c r="A103" s="31"/>
-      <c r="B103" s="38"/>
+      <c r="B103" s="37"/>
       <c r="C103" s="28"/>
       <c r="D103" s="29"/>
       <c r="E103" s="29"/>
@@ -18788,7 +19148,7 @@
     </row>
     <row r="104" ht="34" customHeight="1" spans="1:15">
       <c r="A104" s="31"/>
-      <c r="B104" s="38"/>
+      <c r="B104" s="37"/>
       <c r="C104" s="28"/>
       <c r="D104" s="29"/>
       <c r="E104" s="29"/>
@@ -18805,7 +19165,7 @@
     </row>
     <row r="105" ht="34" customHeight="1" spans="1:15">
       <c r="A105" s="31"/>
-      <c r="B105" s="38"/>
+      <c r="B105" s="37"/>
       <c r="C105" s="28"/>
       <c r="D105" s="29"/>
       <c r="E105" s="29"/>
@@ -18822,7 +19182,7 @@
     </row>
     <row r="106" ht="34" customHeight="1" spans="1:15">
       <c r="A106" s="31"/>
-      <c r="B106" s="38"/>
+      <c r="B106" s="37"/>
       <c r="C106" s="28"/>
       <c r="D106" s="29"/>
       <c r="E106" s="29"/>
@@ -18839,7 +19199,7 @@
     </row>
     <row r="107" ht="34" customHeight="1" spans="1:15">
       <c r="A107" s="31"/>
-      <c r="B107" s="38"/>
+      <c r="B107" s="37"/>
       <c r="C107" s="28"/>
       <c r="D107" s="29"/>
       <c r="E107" s="29"/>
@@ -18856,7 +19216,7 @@
     </row>
     <row r="108" ht="34" customHeight="1" spans="1:15">
       <c r="A108" s="31"/>
-      <c r="B108" s="38"/>
+      <c r="B108" s="37"/>
       <c r="C108" s="28"/>
       <c r="D108" s="29"/>
       <c r="E108" s="29"/>
@@ -18873,7 +19233,7 @@
     </row>
     <row r="109" ht="34" customHeight="1" spans="1:15">
       <c r="A109" s="31"/>
-      <c r="B109" s="38"/>
+      <c r="B109" s="37"/>
       <c r="C109" s="28"/>
       <c r="D109" s="29"/>
       <c r="E109" s="29"/>
@@ -18890,7 +19250,7 @@
     </row>
     <row r="110" ht="34" customHeight="1" spans="1:15">
       <c r="A110" s="31"/>
-      <c r="B110" s="38"/>
+      <c r="B110" s="37"/>
       <c r="C110" s="28"/>
       <c r="D110" s="29"/>
       <c r="E110" s="29"/>
@@ -18907,7 +19267,7 @@
     </row>
     <row r="111" ht="34" customHeight="1" spans="1:15">
       <c r="A111" s="31"/>
-      <c r="B111" s="38"/>
+      <c r="B111" s="37"/>
       <c r="C111" s="33"/>
       <c r="D111" s="30"/>
       <c r="E111" s="30"/>
@@ -18927,7 +19287,7 @@
       <c r="B112" s="23"/>
       <c r="C112" s="28"/>
       <c r="D112" s="29"/>
-      <c r="E112" s="36"/>
+      <c r="E112" s="58"/>
       <c r="F112" s="29"/>
       <c r="G112" s="29"/>
       <c r="H112" s="29"/>
@@ -18945,7 +19305,7 @@
       <c r="B113" s="23"/>
       <c r="C113" s="28"/>
       <c r="D113" s="29"/>
-      <c r="E113" s="36"/>
+      <c r="E113" s="58"/>
       <c r="F113" s="32"/>
       <c r="G113" s="29"/>
       <c r="H113" s="29"/>
@@ -21534,7 +21894,7 @@
     </row>
     <row r="257" ht="23" customHeight="1" spans="1:15">
       <c r="A257" s="31"/>
-      <c r="B257" s="38"/>
+      <c r="B257" s="37"/>
       <c r="C257" s="28"/>
       <c r="D257" s="29"/>
       <c r="E257" s="29"/>
@@ -21551,7 +21911,7 @@
     </row>
     <row r="258" ht="23" customHeight="1" spans="1:15">
       <c r="A258" s="31"/>
-      <c r="B258" s="38"/>
+      <c r="B258" s="37"/>
       <c r="C258" s="28"/>
       <c r="D258" s="29"/>
       <c r="E258" s="29"/>
@@ -21568,7 +21928,7 @@
     </row>
     <row r="259" ht="23" customHeight="1" spans="1:15">
       <c r="A259" s="31"/>
-      <c r="B259" s="38"/>
+      <c r="B259" s="37"/>
       <c r="C259" s="28"/>
       <c r="D259" s="29"/>
       <c r="E259" s="29"/>
@@ -21585,7 +21945,7 @@
     </row>
     <row r="260" ht="23" customHeight="1" spans="1:15">
       <c r="A260" s="31"/>
-      <c r="B260" s="38"/>
+      <c r="B260" s="37"/>
       <c r="C260" s="28"/>
       <c r="D260" s="29"/>
       <c r="E260" s="29"/>
@@ -21602,7 +21962,7 @@
     </row>
     <row r="261" ht="23" customHeight="1" spans="1:15">
       <c r="A261" s="31"/>
-      <c r="B261" s="38"/>
+      <c r="B261" s="37"/>
       <c r="C261" s="28"/>
       <c r="D261" s="29"/>
       <c r="E261" s="29"/>
@@ -21619,7 +21979,7 @@
     </row>
     <row r="262" ht="23" customHeight="1" spans="1:15">
       <c r="A262" s="31"/>
-      <c r="B262" s="38"/>
+      <c r="B262" s="37"/>
       <c r="C262" s="28"/>
       <c r="D262" s="29"/>
       <c r="E262" s="29"/>
@@ -21636,7 +21996,7 @@
     </row>
     <row r="263" ht="23" customHeight="1" spans="1:15">
       <c r="A263" s="31"/>
-      <c r="B263" s="38"/>
+      <c r="B263" s="37"/>
       <c r="C263" s="28"/>
       <c r="D263" s="29"/>
       <c r="E263" s="29"/>
@@ -21653,7 +22013,7 @@
     </row>
     <row r="264" ht="23" customHeight="1" spans="1:15">
       <c r="A264" s="31"/>
-      <c r="B264" s="38"/>
+      <c r="B264" s="37"/>
       <c r="C264" s="28"/>
       <c r="D264" s="29"/>
       <c r="E264" s="29"/>
@@ -21670,7 +22030,7 @@
     </row>
     <row r="265" ht="23" customHeight="1" spans="1:15">
       <c r="A265" s="31"/>
-      <c r="B265" s="38"/>
+      <c r="B265" s="37"/>
       <c r="C265" s="28"/>
       <c r="D265" s="29"/>
       <c r="E265" s="29"/>
@@ -21687,7 +22047,7 @@
     </row>
     <row r="266" ht="23" customHeight="1" spans="1:15">
       <c r="A266" s="31"/>
-      <c r="B266" s="38"/>
+      <c r="B266" s="37"/>
       <c r="C266" s="28"/>
       <c r="D266" s="29"/>
       <c r="E266" s="29"/>
@@ -21704,7 +22064,7 @@
     </row>
     <row r="267" ht="23" customHeight="1" spans="1:15">
       <c r="A267" s="31"/>
-      <c r="B267" s="38"/>
+      <c r="B267" s="37"/>
       <c r="C267" s="28"/>
       <c r="D267" s="29"/>
       <c r="E267" s="29"/>
@@ -21721,7 +22081,7 @@
     </row>
     <row r="268" ht="23" customHeight="1" spans="1:15">
       <c r="A268" s="31"/>
-      <c r="B268" s="38"/>
+      <c r="B268" s="37"/>
       <c r="C268" s="28"/>
       <c r="D268" s="29"/>
       <c r="E268" s="29"/>
@@ -21738,7 +22098,7 @@
     </row>
     <row r="269" ht="23" customHeight="1" spans="1:15">
       <c r="A269" s="31"/>
-      <c r="B269" s="38"/>
+      <c r="B269" s="37"/>
       <c r="C269" s="28"/>
       <c r="D269" s="29"/>
       <c r="E269" s="29"/>
@@ -21755,7 +22115,7 @@
     </row>
     <row r="270" ht="23" customHeight="1" spans="1:15">
       <c r="A270" s="31"/>
-      <c r="B270" s="38"/>
+      <c r="B270" s="37"/>
       <c r="C270" s="28"/>
       <c r="D270" s="29"/>
       <c r="E270" s="29"/>
@@ -21772,7 +22132,7 @@
     </row>
     <row r="271" ht="23" customHeight="1" spans="1:15">
       <c r="A271" s="31"/>
-      <c r="B271" s="38"/>
+      <c r="B271" s="37"/>
       <c r="C271" s="28"/>
       <c r="D271" s="29"/>
       <c r="E271" s="29"/>
@@ -21789,7 +22149,7 @@
     </row>
     <row r="272" ht="23" customHeight="1" spans="1:15">
       <c r="A272" s="31"/>
-      <c r="B272" s="38"/>
+      <c r="B272" s="37"/>
       <c r="C272" s="28"/>
       <c r="D272" s="29"/>
       <c r="E272" s="29"/>
@@ -21806,7 +22166,7 @@
     </row>
     <row r="273" ht="23" customHeight="1" spans="1:15">
       <c r="A273" s="31"/>
-      <c r="B273" s="38"/>
+      <c r="B273" s="37"/>
       <c r="C273" s="28"/>
       <c r="D273" s="29"/>
       <c r="E273" s="29"/>
@@ -21823,7 +22183,7 @@
     </row>
     <row r="274" ht="23" customHeight="1" spans="1:15">
       <c r="A274" s="31"/>
-      <c r="B274" s="38"/>
+      <c r="B274" s="37"/>
       <c r="C274" s="28"/>
       <c r="D274" s="29"/>
       <c r="E274" s="29"/>
@@ -21840,7 +22200,7 @@
     </row>
     <row r="275" ht="23" customHeight="1" spans="1:15">
       <c r="A275" s="31"/>
-      <c r="B275" s="38"/>
+      <c r="B275" s="37"/>
       <c r="C275" s="28"/>
       <c r="D275" s="29"/>
       <c r="E275" s="29"/>
@@ -22007,10 +22367,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C7 C8 C9 C10 C11 C12 C13 C14 C15 C16 C17 C18 C19 C20 C21 C26 C29 C30 C31 C32 C33 C34 C35 C36 C37 C38 C39 C40 C41 C42 C43 C44 C45 C46 C47 C48 C49 C50 C51 C52 C55 C56 C57 C58 C59 C60 C61 C62 C63 C64 C65 C66 C67 C68 C69 C70 C71 C72 C75 C76 C77 C78 C79 C80 C81 C82 C83 C84 C85 C86 C87 C90 C93 C94 C95 C98 C99 C100 C101 C104 C105 C106 C107 C110 C111 C112 C113 C22:C25 C27:C28 C53:C54 C73:C74 C88:C89 C91:C92 C96:C97 C102:C103 C108:C109 C114:C116 C117:C170 C171:C212 C213:C275">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C7 C8 C9 C10 C11 C12 C13 C14 C15 C16 C17 C18 C19 C20 C21 C26 C29 C30 C31 C32 C33 C34 C35 C36 C37 C38 C39 C40 C41 C42 C43 C44 C45 C46 C47 C48 C51 C52 C53 C54 C55 C56 C57 C58 C59 C60 C61 C62 C63 C64 C65 C66 C67 C68 C69 C70 C71 C72 C75 C76 C77 C78 C79 C80 C81 C82 C83 C84 C85 C86 C87 C90 C93 C94 C95 C98 C99 C100 C101 C104 C105 C106 C107 C110 C111 C112 C113 C22:C25 C27:C28 C49:C50 C73:C74 C88:C89 C91:C92 C96:C97 C102:C103 C108:C109 C114:C116 C117:C170 C171:C212 C213:C275">
       <formula1>target</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D26 D29 D30 D31 D32 D33 D34 D35 D36 D37 D38 D39 D40 D41 D42 D43 D44 D45 D46 D47 D48 D49 D50 D51 D52 D55 D56 D57 D58 D59 D60 D61 D62 D63 D64 D65 D66 D67 D68 D69 D70 D71 D72 D75 D76 D77 D78 D79 D80 D81 D82 D83 D84 D85 D86 D87 D90 D91 D92 D93 D94 D95 D98 D99 D100 D101 D104 D105 D106 D107 D110 D111 D112 D113 D6:D7 D22:D25 D27:D28 D53:D54 D73:D74 D88:D89 D96:D97 D102:D103 D108:D109 D114:D116 D117:D159 D160:D275">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D26 D29 D30 D31 D32 D33 D34 D35 D36 D37 D38 D39 D40 D41 D42 D43 D44 D45 D46 D47 D48 D51 D52 D53 D54 D55 D56 D57 D58 D59 D60 D61 D62 D63 D64 D65 D66 D67 D68 D69 D70 D71 D72 D75 D76 D77 D78 D79 D80 D81 D82 D83 D84 D85 D86 D87 D90 D91 D92 D93 D94 D95 D98 D99 D100 D101 D104 D105 D106 D107 D110 D111 D112 D113 D6:D7 D22:D25 D27:D28 D49:D50 D73:D74 D88:D89 D96:D97 D102:D103 D108:D109 D114:D116 D117:D159 D160:D275">
       <formula1>INDIRECT(C5)</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Cash Memo script review comments
</commit_message>
<xml_diff>
--- a/tests/artifact/script/Mobile-CashMemo.xlsx
+++ b/tests/artifact/script/Mobile-CashMemo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6950" tabRatio="550" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="18350" windowHeight="6950" tabRatio="550" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="881">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="883">
   <si>
     <t>target</t>
   </si>
@@ -2706,6 +2706,12 @@
   </si>
   <si>
     <t>Mode of Receipt - Cash and Bank both</t>
+  </si>
+  <si>
+    <t>Verify Product shouldnt be allowed to select if the stock is 0.</t>
+  </si>
+  <si>
+    <t>Validate Purchase Cash Memo section not available.</t>
   </si>
 </sst>
 </file>
@@ -3435,7 +3441,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3640,10 +3646,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -6694,7 +6696,7 @@
   <sheetPr/>
   <dimension ref="A1:P225"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -6861,10 +6863,10 @@
       <c r="O5" s="25"/>
     </row>
     <row r="6" s="3" customFormat="1" ht="15.5" spans="1:15">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="39" t="s">
         <v>750</v>
       </c>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="60" t="s">
         <v>751</v>
       </c>
       <c r="C6" s="33" t="s">
@@ -6876,7 +6878,7 @@
       <c r="E6" s="30" t="s">
         <v>752</v>
       </c>
-      <c r="F6" s="62" t="s">
+      <c r="F6" s="61" t="s">
         <v>753</v>
       </c>
       <c r="G6" s="30"/>
@@ -6891,7 +6893,7 @@
     </row>
     <row r="7" s="4" customFormat="1" ht="42" customHeight="1" spans="1:15">
       <c r="A7" s="22"/>
-      <c r="B7" s="63"/>
+      <c r="B7" s="62"/>
       <c r="C7" s="28"/>
       <c r="D7" s="29"/>
       <c r="E7" s="29"/>
@@ -7297,12 +7299,12 @@
     <row r="31" ht="19" customHeight="1" spans="3:6">
       <c r="C31" s="28"/>
       <c r="D31" s="29"/>
-      <c r="F31" s="64"/>
+      <c r="F31" s="63"/>
     </row>
     <row r="32" ht="19" customHeight="1" spans="3:6">
       <c r="C32" s="28"/>
       <c r="D32" s="29"/>
-      <c r="F32" s="64"/>
+      <c r="F32" s="63"/>
     </row>
     <row r="33" ht="19" customHeight="1" spans="3:6">
       <c r="C33" s="28"/>
@@ -7317,7 +7319,7 @@
     <row r="35" ht="19" customHeight="1" spans="3:6">
       <c r="C35" s="28"/>
       <c r="D35" s="29"/>
-      <c r="F35" s="64"/>
+      <c r="F35" s="63"/>
     </row>
     <row r="36" ht="21" customHeight="1" spans="3:4">
       <c r="C36" s="28"/>
@@ -10769,10 +10771,10 @@
   <sheetPr/>
   <dimension ref="A1:P306"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A54" sqref="A54:A58"/>
+      <selection pane="bottomLeft" activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
@@ -12243,7 +12245,7 @@
       <c r="N54" s="50"/>
       <c r="O54" s="25"/>
     </row>
-    <row r="55" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="55" s="3" customFormat="1" ht="28" spans="1:15">
       <c r="A55" s="39" t="s">
         <v>877</v>
       </c>
@@ -12281,7 +12283,7 @@
       <c r="N56" s="50"/>
       <c r="O56" s="25"/>
     </row>
-    <row r="57" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="57" s="3" customFormat="1" ht="28" spans="1:15">
       <c r="A57" s="39" t="s">
         <v>879</v>
       </c>
@@ -12320,7 +12322,9 @@
       <c r="O58" s="25"/>
     </row>
     <row r="59" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A59" s="31"/>
+      <c r="A59" s="39" t="s">
+        <v>881</v>
+      </c>
       <c r="B59" s="37"/>
       <c r="C59" s="28"/>
       <c r="D59" s="29"/>
@@ -12337,7 +12341,9 @@
       <c r="O59" s="25"/>
     </row>
     <row r="60" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A60" s="31"/>
+      <c r="A60" s="39" t="s">
+        <v>882</v>
+      </c>
       <c r="B60" s="37"/>
       <c r="C60" s="33"/>
       <c r="D60" s="30"/>

</xml_diff>